<commit_message>
Updated timesheet and MOM by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23E66DDB-9BDA-47F4-A9B5-D13638C68A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5CF87D3-F022-4A9B-A4EA-45619708F5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="21-04-22" sheetId="54" r:id="rId13"/>
     <sheet name="22-04-22" sheetId="55" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="408">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1259,6 +1259,9 @@
     <t>visual studio code - .Net SDK is not found in VSCode - Stack Overflow</t>
   </si>
   <si>
+    <t>Dashboard and Layout Responsiveness</t>
+  </si>
+  <si>
     <t>web API(Role)</t>
   </si>
   <si>
@@ -1280,7 +1283,7 @@
     <t>Team discussion-20 min,Meeting with Rafi-60 min,Discussion on Layout-30 min,Team discussion-30 min, Review of service-30 min</t>
   </si>
   <si>
-    <t>Lunch and Break-90 min,Fun friday -1.5 hours, Layout Exploration -1,5 hours</t>
+    <t>Lunch and Break-90 min,Fun friday -2 hours, Layout Exploration -1 hours</t>
   </si>
   <si>
     <t>Web Api exploration</t>
@@ -1309,7 +1312,10 @@
     <t>registration for co-Ordinator</t>
   </si>
   <si>
-    <t>team disussion  -30mim, meeting with rafi-60min,  working on layout for registration page( head)-120min, reviewed the services-35min</t>
+    <t>team disussion  -30mim, meeting with rafi-60min,  working on layout for registration page( head)-90min, reviewed the services-35min</t>
+  </si>
+  <si>
+    <t>lunch -1.15hrs softskill(fun friday activity) with TN team-120min</t>
   </si>
   <si>
     <t>Building Api for Department Service</t>
@@ -3361,15 +3367,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D3FBA-C93D-4333-B7E1-C7BA11A34680}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="30">
+    <row r="1" spans="1:22" ht="30">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="129.75" customHeight="1">
+    <row r="2" spans="1:22" ht="129.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -3410,11 +3416,11 @@
         <v>384</v>
       </c>
       <c r="G2" s="28"/>
-      <c r="I2" s="42" t="s">
+      <c r="V2" s="42" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51">
+    <row r="3" spans="1:22" ht="51">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
@@ -3433,15 +3439,15 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:9" ht="78.75" customHeight="1">
+    <row r="4" spans="1:22" ht="78.75" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>350</v>
+        <v>386</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>351</v>
+        <v>386</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
@@ -3452,62 +3458,62 @@
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="131.25" customHeight="1">
+    <row r="5" spans="1:22" ht="131.25" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:9" ht="113.25" customHeight="1">
+    <row r="6" spans="1:22" ht="113.25" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" ht="77.25" customHeight="1">
+    <row r="7" spans="1:22" ht="77.25" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9" ht="135" customHeight="1">
+    <row r="8" spans="1:22" ht="135" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
@@ -3517,33 +3523,33 @@
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="95.25" customHeight="1">
+    <row r="9" spans="1:22" ht="95.25" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>372</v>
+        <v>403</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="63.75">
+    <row r="10" spans="1:22" ht="63.75">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3562,7 +3568,7 @@
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:9" ht="63" customHeight="1">
+    <row r="11" spans="1:22" ht="63" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
@@ -3581,28 +3587,28 @@
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="57.75" customHeight="1">
+    <row r="12" spans="1:22" ht="57.75" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{120B6D02-1A0C-47E1-B798-6049D6680E11}"/>
+    <hyperlink ref="V2" r:id="rId1" xr:uid="{120B6D02-1A0C-47E1-B798-6049D6680E11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Gokul Modified TimeSheet for 25-4-2022
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D892F95C-87EA-44FB-AA7F-FC83200B6258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BB309B9-7011-4D47-BB3B-F2BAE722A734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="445">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1434,7 +1434,28 @@
 understanding EF ref code - 3 hr</t>
   </si>
   <si>
+    <t>3hrs</t>
+  </si>
+  <si>
     <t>Team Disscussion - 30mins, Meeting with Rafi - 20mins, Working on Head Layout 120mins</t>
+  </si>
+  <si>
+    <t>Common Layout of TMS</t>
+  </si>
+  <si>
+    <t>Common login for TMS and refining the layout</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi - 20mins, Team discussion-20 min,Working on Login layout-60 min,Team discussion-30 min</t>
+  </si>
+  <si>
+    <t>Lunch and Break-90 min</t>
+  </si>
+  <si>
+    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service</t>
+  </si>
+  <si>
+    <t>lunch and breaks - 90mins</t>
   </si>
 </sst>
 </file>
@@ -3992,7 +4013,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4057,8 +4078,12 @@
         <v>436</v>
       </c>
       <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
+      <c r="E3" s="43" t="s">
+        <v>437</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>351</v>
+      </c>
       <c r="G3" s="44"/>
     </row>
     <row r="4" spans="1:7" ht="74.25" customHeight="1">
@@ -4073,7 +4098,7 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>390</v>
@@ -4102,15 +4127,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="C6" s="14"/>
+        <v>439</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>440</v>
+      </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>423</v>
+        <v>442</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -4118,17 +4145,11 @@
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>424</v>
-      </c>
+      <c r="B7" s="23"/>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>426</v>
-      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="138" customHeight="1">
@@ -4203,10 +4224,10 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="G12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Timesheet and MOM updated by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21D256B8-856F-4F45-9476-B261AEAB477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE15C158-7294-4414-8999-3C8664BA9539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="21-04-22" sheetId="54" r:id="rId13"/>
     <sheet name="22-04-22" sheetId="55" r:id="rId14"/>
     <sheet name="23-04-22" sheetId="56" r:id="rId15"/>
+    <sheet name="25-04-22" sheetId="57" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="453">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1145,6 +1146,16 @@
     <t>exploring on web api(2 hrs),break-40 mins,total -2hrs 40 mins</t>
   </si>
   <si>
+    <t>Team meeting -30 min , 
+Client meeting - 60 mins ,
+Team meeting - 30mins,
+Services and classes - 2 hrs, 
+Angular - 3 hrs</t>
+  </si>
+  <si>
+    <t>4hrs</t>
+  </si>
+  <si>
     <t>Layout for TMS except Head navbar</t>
   </si>
   <si>
@@ -1260,13 +1271,13 @@
     <t>visual studio code - .Net SDK is not found in VSCode - Stack Overflow</t>
   </si>
   <si>
-    <t>Dashboard and Layout Responsiveness</t>
-  </si>
-  <si>
-    <t>Team Discussion about Work progress - 20mins, Meeting with Rafi - 60mins, Working and  Alteration on Head Dashboard 120mins</t>
-  </si>
-  <si>
-    <t>Lunch and Tea break-75min , Fun Friday Activity - 90mins</t>
+    <t>Footer, Head View pages(list of coordinator, trainer, trainee, reviewer)</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi - 60mins, Working on Head Layout 120mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunch and Tea break-75min </t>
   </si>
   <si>
     <t>web API(Role)</t>
@@ -1325,6 +1336,24 @@
     <t>lunch -1.15hrs softskill(fun friday activity) with TN team-120min</t>
   </si>
   <si>
+    <t>refining system architecture,review the services</t>
+  </si>
+  <si>
+    <t>1hr : Meeting with Rafi,20 mins : Team Meeting, 35 mins : Review the Services</t>
+  </si>
+  <si>
+    <t>1.30 mins Fun friday,1.30 mins : lunch and break</t>
+  </si>
+  <si>
+    <t>Refining Head dashboard,reviewing services</t>
+  </si>
+  <si>
+    <t>Team discussion -30 min,Meeting with Rafi - 1hr, Working on Head Layout -30 mins, Review the services-20 mins.</t>
+  </si>
+  <si>
+    <t>Lunch -35mins,Break-20 min,fun friday-1.30 min</t>
+  </si>
+  <si>
     <t>Building Api for Department Service</t>
   </si>
   <si>
@@ -1337,16 +1366,120 @@
     <t>lunch and others 90mins, Softskill session - 2hr</t>
   </si>
   <si>
-    <t xml:space="preserve">Team meeting -30 min , Client meeting - 60 mins ,1hr : review the all Layout and clarifying the doubt </t>
+    <t>Meeting with Rafi-60mins,web api department-4hrs</t>
+  </si>
+  <si>
+    <t>Exploring Web api 1 hr,Break 40 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 mins : Team meeting  ,  60 mins:Client meeting ,1hr : review the all Layout and clarifying the doubt </t>
   </si>
   <si>
     <t xml:space="preserve">30 mins : lunch and break time </t>
   </si>
   <si>
+    <t>Meeting with Rafi - 60mins, Working on layout for login and refining the training head-120mins</t>
+  </si>
+  <si>
+    <t>Lunch and Break-90 min,HTML exploration-60  min</t>
+  </si>
+  <si>
+    <t>Web API exploration ,Model for TMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meeting with Rafi - 1 hour, Web Api tutorial - 1 hour , Worked on namespace ,classes and properties-1hr</t>
+  </si>
+  <si>
+    <t>Lunch and break - 1 hour 30 mins</t>
+  </si>
+  <si>
+    <t>exploration on web api,Creating Model for TMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Review Meeting with Rafi-1hr
+web api (exploration)-2hr
+Creating Namespace ,classes and properties in VS code - 1hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Lunch &amp; Tea break - 1.5 hr
+</t>
+  </si>
+  <si>
+    <t>profile page for training head and refining all layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> meeting with rafi-60min,  working on layout for  co ordinator-120min</t>
+  </si>
+  <si>
     <t>Department Service Api</t>
   </si>
   <si>
-    <t>Team meeting -30 min , Client meeting - 60 mins ,Updating MOM - 15min, Design pattern - 55 mins, Adding (Context,Controller,Httpverbs) in department service</t>
+    <t>Team meeting -30 min , Client meeting - 60 mins ,Updating MOM - 15min,  Adding (Context,Controller,Httpverbs) in department service</t>
+  </si>
+  <si>
+    <t>lunch and breaks - 90mins,Design pattern - 55 mins,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Meeting-30 mins,Meeting with Rafi-23mins,web api department-3hrs,total 3 hrs 53 mins </t>
+  </si>
+  <si>
+    <t>collecting System Issues in Corvus 40 mins,Exploring Web api 1 hr,Break 40 mins,relocating my system from caelum  to corvus-40 mins,total 3 hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation
+web api
+</t>
+  </si>
+  <si>
+    <t>team meeting - 30 mins
+web api middleware exploration - 1 hr 30 mins
+meeting with rafi - 20 mins
+team meeting - 30 mins
+understanding EF ref code - 3 hr</t>
+  </si>
+  <si>
+    <t>3hrs</t>
+  </si>
+  <si>
+    <t>Filter, Refining all pages and responsiveness</t>
+  </si>
+  <si>
+    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins</t>
+  </si>
+  <si>
+    <t>Common Layout of TMS</t>
+  </si>
+  <si>
+    <t>Common login for TMS and refining the layout</t>
+  </si>
+  <si>
+    <t>Meeting with Rafi - 20mins, Team discussion-20 min,Working on Login layout-60 min,Team discussion-30 min</t>
+  </si>
+  <si>
+    <t>Lunch and Break-90 min</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Course Topic and Assign course) - 2 hours</t>
+  </si>
+  <si>
+    <t>Others(Lunch and break) - 1 hour 30 mins, Tutorial about HTML</t>
+  </si>
+  <si>
+    <t>HTML layout for confirmation message box</t>
+  </si>
+  <si>
+    <t>Team  meeting-20mins
+Review Meeting with Rafi-20mins
+team discussion -30 mins
+HTML layout (attendance,confirmation message box)-3.5hrs</t>
+  </si>
+  <si>
+    <t>course register page of co-ordinator</t>
+  </si>
+  <si>
+    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service - 4hrs</t>
   </si>
   <si>
     <t>lunch and breaks - 90mins</t>
@@ -1598,7 +1731,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1716,6 +1849,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1726,13 +1871,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2949,14 +3106,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3149,13 +3306,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE4816C-CAE5-4525-AB01-5036960B55BC}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3201,22 +3359,22 @@
       </c>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" spans="1:7" ht="53.25">
+    <row r="3" spans="1:7" ht="90.75" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>289</v>
+      <c r="C3" s="14" t="s">
+        <v>350</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="35" t="s">
-        <v>290</v>
+        <v>351</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>291</v>
+        <v>351</v>
       </c>
       <c r="G3" s="4"/>
     </row>
@@ -3225,17 +3383,17 @@
         <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -3244,36 +3402,36 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="53.25">
+    <row r="6" spans="1:7" ht="51">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -3282,17 +3440,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -3304,14 +3462,14 @@
         <v>302</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -3320,17 +3478,17 @@
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -3339,17 +3497,17 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="35" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -3361,14 +3519,14 @@
         <v>319</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -3377,17 +3535,17 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -3400,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D3FBA-C93D-4333-B7E1-C7BA11A34680}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:G12"/>
+    <sheetView topLeftCell="J5" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
@@ -3445,34 +3603,28 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G2" s="28"/>
       <c r="V2" s="42" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="51">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="35" t="s">
-        <v>290</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="B3" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -3482,14 +3634,14 @@
         <v>319</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -3498,17 +3650,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="G5" s="29"/>
     </row>
@@ -3517,17 +3669,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -3536,15 +3688,15 @@
         <v>20</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -3558,10 +3710,10 @@
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G8" s="4"/>
     </row>
@@ -3570,36 +3722,36 @@
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="63.75">
+    <row r="10" spans="1:22" ht="38.25">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="35" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>376</v>
+        <v>409</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>410</v>
       </c>
       <c r="G10" s="4"/>
     </row>
@@ -3611,14 +3763,14 @@
         <v>319</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>359</v>
+        <v>411</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>378</v>
+        <v>413</v>
       </c>
       <c r="G11" s="4"/>
     </row>
@@ -3627,21 +3779,24 @@
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:G3"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1" xr:uid="{120B6D02-1A0C-47E1-B798-6049D6680E11}"/>
   </hyperlinks>
@@ -3653,14 +3808,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B509DB2-7281-4C29-BE82-B5795AEB1608}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
@@ -3691,6 +3846,235 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="25.5">
+      <c r="A2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>419</v>
+      </c>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" ht="70.5" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="1:7" ht="51">
+      <c r="A4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" ht="53.25" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="35" t="s">
+        <v>420</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>421</v>
+      </c>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" ht="93.75" customHeight="1">
+      <c r="A6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="106.5" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>426</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="138" customHeight="1">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="35" t="s">
+        <v>428</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="133.5" customHeight="1">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="55"/>
+    </row>
+    <row r="11" spans="1:7" ht="36.75" customHeight="1">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
+    </row>
+    <row r="12" spans="1:7" ht="84" customHeight="1">
+      <c r="A12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45">
+      <c r="A1" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" ht="63.75">
       <c r="A2" s="16" t="s">
         <v>9</v>
@@ -3698,197 +4082,190 @@
       <c r="B2" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>347</v>
-      </c>
+      <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>383</v>
+        <v>435</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>384</v>
+        <v>436</v>
       </c>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="91.5" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>298</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-    </row>
-    <row r="4" spans="1:7" ht="51">
+        <v>437</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43" t="s">
+        <v>439</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>351</v>
+      </c>
+      <c r="G3" s="44"/>
+    </row>
+    <row r="4" spans="1:7" ht="74.25" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="45" t="s">
         <v>319</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>386</v>
+        <v>440</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>387</v>
+        <v>441</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" ht="38.25">
+    <row r="5" spans="1:7" ht="53.25" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="165.75">
+    <row r="6" spans="1:7" ht="93.75" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>394</v>
+        <v>443</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>395</v>
+        <v>444</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>396</v>
+        <v>445</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="178.5">
+    <row r="7" spans="1:7" ht="106.5" customHeight="1">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>397</v>
-      </c>
+      <c r="B7" s="23"/>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>398</v>
+        <v>446</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>399</v>
+        <v>447</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="357">
+    <row r="8" spans="1:7" ht="138" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>448</v>
+      </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>400</v>
+        <v>449</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>401</v>
+        <v>429</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="165.75">
+    <row r="9" spans="1:7" ht="133.5" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>402</v>
+        <v>319</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>403</v>
+        <v>450</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>404</v>
+        <v>431</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>405</v>
+        <v>374</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="204">
+    <row r="10" spans="1:7" ht="35.25" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>373</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="35" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="191.25">
+      <c r="B10" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="55"/>
+    </row>
+    <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>359</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
-        <v>377</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="68.25" customHeight="1">
+      <c r="B11" s="53" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="55"/>
+    </row>
+    <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>413</v>
+        <v>451</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>414</v>
+        <v>452</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:G3"/>
+  <mergeCells count="2">
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated timesheet by ragu
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C267D55F-A2BA-48C1-B8C0-05074F08E65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{59816D3B-6098-4A43-923A-A735DFFFE996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="458">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1410,7 +1410,7 @@
     <t>profile page for training head and refining all layout</t>
   </si>
   <si>
-    <t xml:space="preserve"> meeting with rafi-60min,  working on layout for  co ordinator-120min</t>
+    <t xml:space="preserve"> team discussion-20min,meeting with rafi-23min, team discussion-30min(abouth the layout completion)  working on layout for  profile view page (training head) -120min</t>
   </si>
   <si>
     <t>Department Service Api</t>
@@ -1443,10 +1443,25 @@
     <t>3hrs</t>
   </si>
   <si>
-    <t>Filter, Refining all pages and responsiveness</t>
-  </si>
-  <si>
-    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins</t>
+    <t>Filter, Search , Refining all pages and responsiveness</t>
+  </si>
+  <si>
+    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins, alteration in signin, signup page</t>
+  </si>
+  <si>
+    <t>Lunch and Break-75 min</t>
+  </si>
+  <si>
+    <t>Home page Layout</t>
+  </si>
+  <si>
+    <t>Entire MOM Layout</t>
+  </si>
+  <si>
+    <t>30 mins : Team meeting  ,  20 mins:Client meeting,30mins : Team discussion in Layout Completion, 1.30 mins MoM layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.30 mins : lunch and break time </t>
   </si>
   <si>
     <t>Common Layout of TMS</t>
@@ -1461,10 +1476,13 @@
     <t>Lunch and Break-90 min</t>
   </si>
   <si>
-    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Course Topic and Assign course) - 2 hours</t>
-  </si>
-  <si>
-    <t>Others(Lunch and break) - 1 hour 30 mins</t>
+    <t>Working on  Responsiveness for Create Topic page</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Create Topic and Assign course) - 2 hours</t>
+  </si>
+  <si>
+    <t>Others(Lunch and break) - 1 hour 30 mins, Tutorial about HTML - 1 hour</t>
   </si>
   <si>
     <t>HTML layout for confirmation message box</t>
@@ -1476,10 +1494,7 @@
 HTML layout (attendance,confirmation message box)-3.5hrs</t>
   </si>
   <si>
-    <t>course register page of co-ordinator</t>
-  </si>
-  <si>
-    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service</t>
+    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service - 4hrs</t>
   </si>
   <si>
     <t>lunch and breaks - 90mins</t>
@@ -1731,7 +1746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1863,6 +1878,15 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3106,14 +3130,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3617,14 +3641,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="54" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -3809,7 +3833,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3867,14 +3891,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="54" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="1:7" ht="51">
       <c r="A4" s="16" t="s">
@@ -3984,27 +4008,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4037,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4125,8 +4149,8 @@
       <c r="E4" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>390</v>
+      <c r="F4" s="19" t="s">
+        <v>442</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -4135,15 +4159,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="14"/>
+        <v>443</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>444</v>
+      </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="G5" s="29"/>
     </row>
@@ -4152,17 +4178,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -4170,14 +4196,16 @@
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="23" t="s">
+        <v>451</v>
+      </c>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -4189,11 +4217,11 @@
         <v>302</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>429</v>
@@ -4204,11 +4232,9 @@
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>319</v>
-      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
@@ -4223,27 +4249,23 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
-    </row>
-    <row r="11" spans="1:7" ht="36.75" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="54" t="s">
-        <v>298</v>
-      </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+    </row>
+    <row r="11" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4255,17 +4277,16 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
gokul updated time sheet for 26-4-2022
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25216"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BB309B9-7011-4D47-BB3B-F2BAE722A734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{24087D29-89FC-40D5-B61F-689E15182F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="22-04-22" sheetId="55" r:id="rId14"/>
     <sheet name="23-04-22" sheetId="56" r:id="rId15"/>
     <sheet name="25-04-22" sheetId="57" r:id="rId16"/>
+    <sheet name="26-04-22" sheetId="58" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="480">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1407,10 +1408,10 @@
 </t>
   </si>
   <si>
-    <t>course register page of co-ordinator</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> meeting with rafi-60min,  working on layout for  co ordinator-120min</t>
+    <t>profile page for training head and refining all layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> team discussion-20min,meeting with rafi-23min, team discussion-30min(abouth the layout completion)  working on layout for  profile view page (training head) -120min</t>
   </si>
   <si>
     <t>Department Service Api</t>
@@ -1420,6 +1421,12 @@
   </si>
   <si>
     <t>lunch and breaks - 90mins,Design pattern - 55 mins,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Meeting-30 mins,Meeting with Rafi-23mins,web api department-3hrs,total 3 hrs 53 mins </t>
+  </si>
+  <si>
+    <t>collecting System Issues in Corvus 40 mins,Exploring Web api 1 hr,Break 40 mins,relocating my system from caelum  to corvus-40 mins,total 3 hrs</t>
   </si>
   <si>
     <t xml:space="preserve">Estimation
@@ -1437,7 +1444,25 @@
     <t>3hrs</t>
   </si>
   <si>
-    <t>Team Disscussion - 30mins, Meeting with Rafi - 20mins, Working on Head Layout 120mins</t>
+    <t>Filter, Search , Refining all pages and responsiveness</t>
+  </si>
+  <si>
+    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins, alteration in signin, signup page</t>
+  </si>
+  <si>
+    <t>Lunch and Break-75 min</t>
+  </si>
+  <si>
+    <t>Home page Layout</t>
+  </si>
+  <si>
+    <t>Entire MOM Layout</t>
+  </si>
+  <si>
+    <t>30 mins : Team meeting  ,  20 mins:Client meeting,30mins : Team discussion in Layout Completion, 1.30 mins MoM layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.30 mins : lunch and break time </t>
   </si>
   <si>
     <t>Common Layout of TMS</t>
@@ -1452,17 +1477,153 @@
     <t>Lunch and Break-90 min</t>
   </si>
   <si>
-    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service</t>
+    <t>Working on  Responsiveness for Create Topic page</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Create Topic and Assign course) - 2 hours</t>
+  </si>
+  <si>
+    <t>Others(Lunch and break) - 1 hour 30 mins, Tutorial about HTML - 1 hour</t>
+  </si>
+  <si>
+    <t>HTML layout for confirmation message box</t>
+  </si>
+  <si>
+    <t>Team  meeting-20mins
+Review Meeting with Rafi-20mins
+team discussion -30 mins
+HTML layout (attendance,confirmation message box)-3.5hrs</t>
+  </si>
+  <si>
+    <t>Home Page Layout</t>
+  </si>
+  <si>
+    <t>layout for schedule review and view review for TMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Team meeting for 30 mins  , Client meeting- 20 mins, Team discussion for splitting the work - 30 mins, 1.30 mins for Review page</t>
+  </si>
+  <si>
+    <t>Lunch break - 1:30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainee Feedback layout ,Course Feedback layout </t>
+  </si>
+  <si>
+    <t>Team meeting-20 mins, meeting with client -23 mins,Team meeting( About layout completion)-30 min, working on layout for trainee feedback and course feedback -3h30mins</t>
+  </si>
+  <si>
+    <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service - 4hrs</t>
   </si>
   <si>
     <t>lunch and breaks - 90mins</t>
+  </si>
+  <si>
+    <t>Web Api services</t>
+  </si>
+  <si>
+    <t>8:30 - 9:05(35mins) : Updating timesheet and MOM,
+9:05 - 9:30(25mins) : Team meeting,      
+9:30 - 10:20(50mins) : Softskill,
+10:20 - 10:40(20mins) : break,
+10:45 - 11:45(60mins) : Web api services added(User,Department,Role),  
+11:45 - 12:15(30mins) : Estimation of pages in TMS, 
+12:15 - 12:25(10mins) : Helping in resolve a conflict,
+12:35 - 12:55(20mins) : Client meeting,
+1:00 - 1:40(40mins) : Lunch,
+2:00 - 2:40(40mins) : Web api session among team,  
+2:40 - 3:00(10mins) : worked on a Services,  
+3:00 - 3:40(40mins) : rework on a new repository,                                        
+3:40 - 4:15(35mins) : Implementing Serilog in api,
+4:15 - 4:30(15mins) : break,
+4:30 - 5:15(45mins) : Resolving conflict in webapi,
+5:15 - 5:45(30mins) : Clarifying about repository and worked on new repository
+7:00 - 7:45(45mis) : Midlleware exploration</t>
+  </si>
+  <si>
+    <t>6.3 hrs</t>
+  </si>
+  <si>
+    <t>3.10 hrs</t>
+  </si>
+  <si>
+    <t>Web api (Debugging Errors-(8:15-9:00),                    repository(9:00-9:44),(10:40-12:00) ,                                 Estimation and discussion(12:00-12-33),Meeting with Rafi(12:36-12:52),Timesheet update(2:00-2:15),</t>
+  </si>
+  <si>
+    <t>Softskill session(9:44-10:33),Break(1:05-1:40),sending mail for installation(2:40-2:45),Webapi exploring(3:00-3:30),college call(3:30-3:45),Break(3:45-4:00),System installation (4:00-4:25),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Api exploration,
+Ef Core exploration
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00 - 9:20 : TimeSheet,
+9:20 - 9:35 : Team meeting,      
+9:35 - 10:20 : Softskill,
+10:20 - 10:40 : Break,   
+10:40 - 10:55 : Estimation explaination,
+10:55 - 11:45 : Web api services added(DbContext,Migrations,UserService), 
+11:45 - 12:35 : Estimation of pages in TMS, 
+12:35 - 12:56 : Client meeting,
+12:56 - 1:30 : Lunch
+1:30 - 2:00 : preparing for web api session 
+2:00 - 3:00 : worked on UserServices.cs,
+3:00 - 4:00 : Web api session among team,                                         
+4:00 - 4:30 : worked on IRepository.cs,
+4:30 - 4:45 : Break,
+4:45 - 5:30 : Resolving conflict in Webapi </t>
+  </si>
+  <si>
+    <t>Estimation and Layout Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet and HLD Document
+9:05 - 9:30 : Team meeting
+10:40-10:55 : Estimation explanation meeting
+11:00-11:30 : Integrating my MOM layout with other layout pages 
+11.30-12.15: Helping in Attendence Layout
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 mins : Identifying the pages and Estimation
+4.35-4.50 : Web API Session with other team 
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 : Softskill
+3:00 - 4:00: webAPI Session with team
+10:20 - 10:40 : break
+1:00 - 1:40 : Lunch
+4:00- 4:15 : break</t>
+  </si>
+  <si>
+    <t>Refining the layout and responvise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation explanation meeting-15 min
+30mins : Helping in Attendence Layout
+15 mins : meeting with Rafi 
+1.30 mins : Estimation
+10 mins : Layout Correction Explanation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softskill-1 hour
+webAPI Session with team-1 hour, Prepare for Review -100 mins
+lunch and Break-80 mins </t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 - Softskill session</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1599,6 +1760,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1608,7 +1776,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1699,12 +1867,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1828,6 +2011,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1855,14 +2065,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3079,14 +3348,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3197,7 +3466,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:10" ht="37.5">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
@@ -3290,7 +3559,7 @@
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3313,7 +3582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63.75">
+    <row r="2" spans="1:7" ht="74.25">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3658,7 @@
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="51">
+    <row r="6" spans="1:7" ht="49.5">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
@@ -3408,7 +3677,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="51">
+    <row r="7" spans="1:7" ht="49.5">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -3465,7 +3734,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="89.25">
+    <row r="10" spans="1:7" ht="61.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3531,8 +3800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D3FBA-C93D-4333-B7E1-C7BA11A34680}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="J5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
@@ -3541,7 +3810,7 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30">
+    <row r="1" spans="1:22">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3590,14 +3859,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -3709,7 +3978,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="38.25">
+    <row r="10" spans="1:22" ht="25.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3781,8 +4050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B509DB2-7281-4C29-BE82-B5795AEB1608}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3796,7 +4065,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3840,16 +4109,16 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
-    </row>
-    <row r="4" spans="1:7" ht="51">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+    </row>
+    <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
@@ -3940,9 +4209,7 @@
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>319</v>
-      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
         <v>430</v>
       </c>
@@ -3959,27 +4226,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4013,7 +4280,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4027,7 +4294,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -4050,7 +4317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5">
+    <row r="2" spans="1:7" ht="61.5">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -4060,10 +4327,10 @@
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="13" t="s">
-        <v>418</v>
+        <v>435</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>419</v>
+        <v>436</v>
       </c>
       <c r="G2" s="28"/>
     </row>
@@ -4071,15 +4338,15 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>435</v>
-      </c>
-      <c r="C3" s="56" t="s">
-        <v>436</v>
+      <c r="B3" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>438</v>
       </c>
       <c r="D3" s="43"/>
       <c r="E3" s="43" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>351</v>
@@ -4090,18 +4357,18 @@
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="48" t="s">
         <v>319</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>388</v>
+        <v>440</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14" t="s">
-        <v>438</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>390</v>
+        <v>441</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>442</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -4110,15 +4377,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="14"/>
+        <v>443</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>444</v>
+      </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="G5" s="29"/>
     </row>
@@ -4127,17 +4396,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -4145,11 +4414,17 @@
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="23" t="s">
+        <v>451</v>
+      </c>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>453</v>
+      </c>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="138" customHeight="1">
@@ -4157,12 +4432,14 @@
         <v>21</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="C8" s="14"/>
+        <v>302</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>454</v>
+      </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>429</v>
@@ -4173,9 +4450,7 @@
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>319</v>
-      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
         <v>430</v>
       </c>
@@ -4188,31 +4463,40 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+    <row r="10" spans="1:7" ht="55.5" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="51" t="s">
-        <v>298</v>
-      </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="53"/>
-    </row>
-    <row r="11" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B10" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>457</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="35" t="s">
+        <v>458</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="79.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>298</v>
-      </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4224,18 +4508,254 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>443</v>
+        <v>462</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>444</v>
+        <v>463</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7172FC-5606-4FD6-B7B3-02AB5BD496A0}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" style="65"/>
+    <col min="2" max="2" width="30.28515625" style="65" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="65" customWidth="1"/>
+    <col min="4" max="4" width="25" style="65"/>
+    <col min="5" max="5" width="47" style="65" customWidth="1"/>
+    <col min="6" max="6" width="42" style="65" customWidth="1"/>
+    <col min="7" max="16384" width="25" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="66" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="267" customHeight="1">
+      <c r="A2" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>465</v>
+      </c>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>467</v>
+      </c>
+      <c r="G2" s="82"/>
+    </row>
+    <row r="3" spans="1:7" ht="89.25">
+      <c r="A3" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69" t="s">
+        <v>468</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>469</v>
+      </c>
+      <c r="G3" s="83"/>
+    </row>
+    <row r="4" spans="1:7" ht="244.5" customHeight="1">
+      <c r="A4" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>471</v>
+      </c>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="G4" s="64"/>
+    </row>
+    <row r="5" spans="1:7" ht="133.5" customHeight="1">
+      <c r="A5" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>440</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68" t="s">
+        <v>441</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>442</v>
+      </c>
+      <c r="G5" s="63"/>
+    </row>
+    <row r="6" spans="1:7" ht="150" customHeight="1">
+      <c r="A6" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="68" t="s">
+        <v>472</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>474</v>
+      </c>
+      <c r="G6" s="84"/>
+    </row>
+    <row r="7" spans="1:7" ht="132.75" customHeight="1">
+      <c r="A7" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" s="68"/>
+      <c r="E7" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>477</v>
+      </c>
+      <c r="G7" s="82"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="74"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69" t="s">
+        <v>478</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="1:7" ht="63.75">
+      <c r="A9" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="75" t="s">
+        <v>455</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>429</v>
+      </c>
+      <c r="G9" s="82"/>
+    </row>
+    <row r="10" spans="1:7" ht="75.75" customHeight="1">
+      <c r="A10" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68" t="s">
+        <v>430</v>
+      </c>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68" t="s">
+        <v>431</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>374</v>
+      </c>
+      <c r="G10" s="82"/>
+    </row>
+    <row r="11" spans="1:7" ht="144" customHeight="1">
+      <c r="A11" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>456</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>457</v>
+      </c>
+      <c r="D11" s="77"/>
+      <c r="E11" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="141.75" customHeight="1">
+      <c r="A12" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>479</v>
+      </c>
+      <c r="G12" s="85"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated timesheet and MOM sheet by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25216"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE15C158-7294-4414-8999-3C8664BA9539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66BF6169-7F24-419C-BE45-FC83F4CF5173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="22-04-22" sheetId="55" r:id="rId14"/>
     <sheet name="23-04-22" sheetId="56" r:id="rId15"/>
     <sheet name="25-04-22" sheetId="57" r:id="rId16"/>
+    <sheet name="26-04-22" sheetId="58" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="480">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1410,7 +1411,7 @@
     <t>profile page for training head and refining all layout</t>
   </si>
   <si>
-    <t xml:space="preserve"> meeting with rafi-60min,  working on layout for  co ordinator-120min</t>
+    <t xml:space="preserve"> team discussion-20min,meeting with rafi-23min, team discussion-30min(abouth the layout completion)  working on layout for  profile view page (training head) -120min</t>
   </si>
   <si>
     <t>Department Service Api</t>
@@ -1443,10 +1444,25 @@
     <t>3hrs</t>
   </si>
   <si>
-    <t>Filter, Refining all pages and responsiveness</t>
-  </si>
-  <si>
-    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins</t>
+    <t>Filter, Search , Refining all pages and responsiveness</t>
+  </si>
+  <si>
+    <t>Team Discussion - 20mins, Meeting with Rafi - 20mins, Team Discussion about Layout Completion -30mins, alteration in signin, signup page</t>
+  </si>
+  <si>
+    <t>Lunch and Break-75 min</t>
+  </si>
+  <si>
+    <t>Home page Layout</t>
+  </si>
+  <si>
+    <t>Entire MOM Layout</t>
+  </si>
+  <si>
+    <t>30 mins : Team meeting  ,  20 mins:Client meeting,30mins : Team discussion in Layout Completion, 1.30 mins MoM layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.30 mins : lunch and break time </t>
   </si>
   <si>
     <t>Common Layout of TMS</t>
@@ -1461,10 +1477,13 @@
     <t>Lunch and Break-90 min</t>
   </si>
   <si>
-    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Course Topic and Assign course) - 2 hours</t>
-  </si>
-  <si>
-    <t>Others(Lunch and break) - 1 hour 30 mins, Tutorial about HTML</t>
+    <t>Working on  Responsiveness for Create Topic page</t>
+  </si>
+  <si>
+    <t>Team meeting - 30 mins, Meeting with Rafi - 20 mins , Created a layout page (Create Topic and Assign course) - 2 hours</t>
+  </si>
+  <si>
+    <t>Others(Lunch and break) - 1 hour 30 mins, Tutorial about HTML - 1 hour</t>
   </si>
   <si>
     <t>HTML layout for confirmation message box</t>
@@ -1476,20 +1495,135 @@
 HTML layout (attendance,confirmation message box)-3.5hrs</t>
   </si>
   <si>
-    <t>course register page of co-ordinator</t>
+    <t>Home Page Layout</t>
+  </si>
+  <si>
+    <t>layout for schedule review and view review for TMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Team meeting for 30 mins  , Client meeting- 20 mins, Team discussion for splitting the work - 30 mins, 1.30 mins for Review page</t>
+  </si>
+  <si>
+    <t>Lunch break - 1:30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainee Feedback layout ,Course Feedback layout </t>
+  </si>
+  <si>
+    <t>Team meeting-20 mins, meeting with client -23 mins,Team meeting( About layout completion)-30 min, working on layout for trainee feedback and course feedback -3h30mins</t>
   </si>
   <si>
     <t>Team meeting -30 min , Client meeting - 20mins ,Updating MOM - 10min,  Creating (CRUD operations) in department service - 4hrs</t>
   </si>
   <si>
     <t>lunch and breaks - 90mins</t>
+  </si>
+  <si>
+    <t>Web Api services</t>
+  </si>
+  <si>
+    <t>8:30 - 9:05(35mins) : Updating timesheet and MOM,
+9:05 - 9:30(25mins) : Team meeting,      
+9:30 - 10:20(50mins) : Softskill,
+10:20 - 10:40(20mins) : break,
+10:45 - 11:45(60mins) : Web api services added(User,Department,Role),  
+11:45 - 12:15(30mins) : Estimation of pages in TMS, 
+12:15 - 12:25(10mins) : Helping in resolve a conflict,
+12:35 - 12:55(20mins) : Client meeting,
+1:00 - 1:40(40mins) : Lunch,
+2:00 - 2:40(40mins) : Web api session among team,  
+2:40 - 3:00(10mins) : worked on a Services,  
+3:00 - 3:40(40mins) : rework on a new repository,                                        
+3:40 - 4:15(35mins) : Implementing Serilog in api,
+4:15 - 4:30(15mins) : break,
+4:30 - 5:15(45mins) : Resolving conflict in webapi,
+5:15 - 5:45(30mins) : Clarifying about repository and worked on new repository
+7:00 - 7:45(45mis) : Midlleware exploration</t>
+  </si>
+  <si>
+    <t>6.3 hrs</t>
+  </si>
+  <si>
+    <t>3.10 hrs</t>
+  </si>
+  <si>
+    <t>Web api (Debugging Errors-(8:15-9:00),                    repository(9:00-9:44),(10:40-12:00) ,                                 Estimation and discussion(12:00-12-33),Meeting with Rafi(12:36-12:52),Timesheet update(2:00-2:15),</t>
+  </si>
+  <si>
+    <t>Softskill session(9:44-10:33),Break(1:05-1:40),sending mail for installation(2:40-2:45),Webapi exploring(3:00-3:30),college call(3:30-3:45),Break(3:45-4:00),System installation (4:00-4:25),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Api exploration,
+Ef Core exploration
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00 - 9:20 : TimeSheet,
+9:20 - 9:35 : Team meeting,      
+9:35 - 10:20 : Softskill,
+10:20 - 10:40 : Break,   
+10:40 - 10:55 : Estimation explaination,
+10:55 - 11:45 : Web api services added(DbContext,Migrations,UserService), 
+11:45 - 12:35 : Estimation of pages in TMS, 
+12:35 - 12:56 : Client meeting,
+12:56 - 1:30 : Lunch
+1:30 - 2:00 : preparing for web api session 
+2:00 - 3:00 : worked on UserServices.cs,
+3:00 - 4:00 : Web api session among team,                                         
+4:00 - 4:30 : worked on IRepository.cs,
+4:30 - 4:45 : Break,
+4:45 - 5:30 : Resolving conflict in Webapi </t>
+  </si>
+  <si>
+    <t>Estimation and Layout Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet and HLD Document
+9:05 - 9:30 : Team meeting
+10:40-10:55 : Estimation explanation meeting
+11:00-11:30 : Integrating my MOM layout with other layout pages 
+11.30-12.15: Helping in Attendence Layout
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 mins : Identifying the pages and Estimation
+4.35-4.50 : Web API Session with other team 
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 : Softskill
+3:00 - 4:00: webAPI Session with team
+10:20 - 10:40 : break
+1:00 - 1:40 : Lunch
+4:00- 4:15 : break</t>
+  </si>
+  <si>
+    <t>Refining the layout and responvise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation explanation meeting
+30mins : Helping in Attendence Layout
+15 mins : meeting with Rafi 
+1.30 mins : Estimation
+10 mins : Layout Correction Explanation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Softskill-1 hour
+webAPI Session with team-1 hour, Prepare for Review -100 mins
+lunch and Break-80 mins </t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 - Softskill session</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1626,6 +1760,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1635,7 +1776,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1726,12 +1867,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1855,12 +2011,33 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1888,8 +2065,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3106,14 +3348,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3224,7 +3466,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:10" ht="37.5">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
@@ -3317,7 +3559,7 @@
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3340,7 +3582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63.75">
+    <row r="2" spans="1:7" ht="74.25">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -3416,7 +3658,7 @@
       </c>
       <c r="G5" s="29"/>
     </row>
-    <row r="6" spans="1:7" ht="51">
+    <row r="6" spans="1:7" ht="49.5">
       <c r="A6" s="30" t="s">
         <v>19</v>
       </c>
@@ -3435,7 +3677,7 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="51">
+    <row r="7" spans="1:7" ht="49.5">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -3492,7 +3734,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="89.25">
+    <row r="10" spans="1:7" ht="61.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3558,8 +3800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2D3FBA-C93D-4333-B7E1-C7BA11A34680}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="J5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15"/>
@@ -3568,7 +3810,7 @@
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30">
+    <row r="1" spans="1:22">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3617,14 +3859,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -3736,7 +3978,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:22" ht="38.25">
+    <row r="10" spans="1:22" ht="25.5">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
@@ -3809,7 +4051,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3823,7 +4065,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -3867,16 +4109,16 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="57" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
-    </row>
-    <row r="4" spans="1:7" ht="51">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+    </row>
+    <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
@@ -3984,27 +4226,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="60" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4037,8 +4279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4052,7 +4294,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7">
       <c r="A1" s="27" t="s">
         <v>258</v>
       </c>
@@ -4075,7 +4317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63.75">
+    <row r="2" spans="1:7" ht="61.5">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -4096,10 +4338,10 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="49" t="s">
         <v>437</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="50" t="s">
         <v>438</v>
       </c>
       <c r="D3" s="43"/>
@@ -4115,7 +4357,7 @@
       <c r="A4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="48" t="s">
         <v>319</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -4125,8 +4367,8 @@
       <c r="E4" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>390</v>
+      <c r="F4" s="19" t="s">
+        <v>442</v>
       </c>
       <c r="G4" s="13"/>
     </row>
@@ -4135,15 +4377,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="14"/>
+        <v>443</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>444</v>
+      </c>
       <c r="D5" s="14"/>
       <c r="E5" s="35" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="G5" s="29"/>
     </row>
@@ -4152,17 +4396,17 @@
         <v>19</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="13" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="G6" s="4"/>
     </row>
@@ -4170,14 +4414,16 @@
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="23" t="s">
+        <v>451</v>
+      </c>
       <c r="C7" s="33"/>
       <c r="D7" s="14"/>
       <c r="E7" s="13" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="G7" s="4"/>
     </row>
@@ -4189,11 +4435,11 @@
         <v>302</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="35" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>429</v>
@@ -4204,11 +4450,9 @@
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>319</v>
-      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
@@ -4219,31 +4463,40 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="35.25" customHeight="1">
+    <row r="10" spans="1:7" ht="55.5" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="53" t="s">
-        <v>298</v>
-      </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:7" ht="36.75" customHeight="1">
+      <c r="B10" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>457</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="35" t="s">
+        <v>458</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>459</v>
+      </c>
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="79.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>298</v>
-      </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4255,18 +4508,250 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="G12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7172FC-5606-4FD6-B7B3-02AB5BD496A0}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25" style="65"/>
+    <col min="2" max="2" width="30.28515625" style="65" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="65" customWidth="1"/>
+    <col min="4" max="4" width="25" style="65"/>
+    <col min="5" max="5" width="47" style="65" customWidth="1"/>
+    <col min="6" max="6" width="42" style="65" customWidth="1"/>
+    <col min="7" max="16384" width="25" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="66" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="267" customHeight="1">
+      <c r="A2" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>465</v>
+      </c>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>467</v>
+      </c>
+      <c r="G2" s="82"/>
+    </row>
+    <row r="3" spans="1:7" ht="89.25">
+      <c r="A3" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69" t="s">
+        <v>468</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>469</v>
+      </c>
+      <c r="G3" s="83"/>
+    </row>
+    <row r="4" spans="1:7" ht="244.5" customHeight="1">
+      <c r="A4" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>470</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>471</v>
+      </c>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="G4" s="64"/>
+    </row>
+    <row r="5" spans="1:7" ht="133.5" customHeight="1">
+      <c r="A5" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>440</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68" t="s">
+        <v>441</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>442</v>
+      </c>
+      <c r="G5" s="63"/>
+    </row>
+    <row r="6" spans="1:7" ht="120" customHeight="1">
+      <c r="A6" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="74"/>
+      <c r="C6" s="68" t="s">
+        <v>472</v>
+      </c>
+      <c r="D6" s="68"/>
+      <c r="E6" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>474</v>
+      </c>
+      <c r="G6" s="84"/>
+    </row>
+    <row r="7" spans="1:7" ht="132.75" customHeight="1">
+      <c r="A7" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" s="68"/>
+      <c r="E7" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>477</v>
+      </c>
+      <c r="G7" s="82"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="74"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69" t="s">
+        <v>478</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="1:7" ht="63.75">
+      <c r="A9" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="75" t="s">
+        <v>455</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>429</v>
+      </c>
+      <c r="G9" s="82"/>
+    </row>
+    <row r="10" spans="1:7" ht="75.75" customHeight="1">
+      <c r="A10" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68" t="s">
+        <v>430</v>
+      </c>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68" t="s">
+        <v>431</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>374</v>
+      </c>
+      <c r="G10" s="82"/>
+    </row>
+    <row r="11" spans="1:7" ht="144" customHeight="1">
+      <c r="A11" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="77"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="F11" s="75" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="141.75" customHeight="1">
+      <c r="A12" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="79" t="s">
+        <v>461</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>479</v>
+      </c>
+      <c r="G12" s="85"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated timesheet by sobhana M
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BCAAEB8-CB95-4956-A755-6AF5DE8A7A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81E8CC98-168F-4207-AE08-DCCCCAC1378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="495">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1702,16 +1702,22 @@
 4:00-4:30   : Tea Break</t>
   </si>
   <si>
-    <t>8.45-9.00    : Updating Timesheet
+    <t xml:space="preserve">8.45-9.00    : Updating Timesheet
 9:00 - 9:30  : Team meeting
 10:40-10:55  : Estimation explanation meeting
-11:00-11:45  : Refining Feedback layout, integrating with other layouts and updating in git 
+11:00-11:45  : Refining Feedback layout, intergrating with other layouts and updating in git 
 11.45-12.15  : Helping in Estimation
 12:35 - 12:56: meeting with Rafi 
 2.00-3.00    : Identifying the pages and Estimation
-3.00-4.00    : Web API Session with other team 
-4.30-4.50    : Exploring web api and installing packages
-4.55- 5.45   : Layout Correction and Estimation layout pages</t>
+3.00-4.00    : Web API Session with team 
+4.30-4.50    : Web API Session with other team 
+4.55- 5.45   : Exploring web api and installing packages ,Estimationing layout pages
+</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 : Softskill
+10.20 -10.40 : Break
+1.00-1.40    : Lunch</t>
   </si>
   <si>
     <t>Estimation for TMS and refineed layouts</t>
@@ -2218,38 +2224,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3466,14 +3472,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3977,14 +3983,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="82"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -4227,14 +4233,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="82"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="16" t="s">
@@ -4344,27 +4350,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="85"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="83"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="81" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="85"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="83"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4397,8 +4403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:G12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4642,8 +4648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7172FC-5606-4FD6-B7B3-02AB5BD496A0}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25" defaultRowHeight="15"/>
@@ -4746,7 +4752,7 @@
       <c r="E5" s="58" t="s">
         <v>473</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="85" t="s">
         <v>474</v>
       </c>
       <c r="G5" s="54"/>
@@ -4792,7 +4798,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="65"/>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="84" t="s">
         <v>481</v>
       </c>
       <c r="D8" s="58"/>
@@ -4852,7 +4858,9 @@
       <c r="E11" s="64" t="s">
         <v>490</v>
       </c>
-      <c r="F11" s="64"/>
+      <c r="F11" s="64" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="141.75" customHeight="1">
       <c r="A12" s="57" t="s">
@@ -4860,14 +4868,14 @@
       </c>
       <c r="B12" s="66"/>
       <c r="C12" s="67" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D12" s="66"/>
       <c r="E12" s="68" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="G12" s="74"/>
     </row>

</xml_diff>

<commit_message>
gokul updated time sheet for 27-4-2022
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24087D29-89FC-40D5-B61F-689E15182F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{959B22BE-18E2-4D2B-B840-21C6ADB984B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5-4-22" sheetId="40" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="23-04-22" sheetId="56" r:id="rId15"/>
     <sheet name="25-04-22" sheetId="57" r:id="rId16"/>
     <sheet name="26-04-22" sheetId="58" r:id="rId17"/>
+    <sheet name="27-04-22" sheetId="59" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="563">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1547,10 +1548,16 @@
     <t>3.10 hrs</t>
   </si>
   <si>
-    <t>Web api (Debugging Errors-(8:15-9:00),                    repository(9:00-9:44),(10:40-12:00) ,                                 Estimation and discussion(12:00-12-33),Meeting with Rafi(12:36-12:52),Timesheet update(2:00-2:15),</t>
-  </si>
-  <si>
-    <t>Softskill session(9:44-10:33),Break(1:05-1:40),sending mail for installation(2:40-2:45),Webapi exploring(3:00-3:30),college call(3:30-3:45),Break(3:45-4:00),System installation (4:00-4:25),</t>
+    <t>web api Services and web api exploration</t>
+  </si>
+  <si>
+    <t>20:00-21:00 : reviewing and understanding the Api services,
+21:00-23:00 : Learning Angular&lt;Components and lifecycle&gt;,
+TOTAL-3 hrs</t>
+  </si>
+  <si>
+    <t>8:00-17:00 : Went college for internals ,
+TOTAL -9 hrs</t>
   </si>
   <si>
     <t xml:space="preserve">Web Api exploration,
@@ -1575,6 +1582,27 @@
 4:45 - 5:30 : Resolving conflict in Webapi </t>
   </si>
   <si>
+    <t>Component in angular for common Layout pages</t>
+  </si>
+  <si>
+    <t>8.40-9.00   : Updating Timesheet
+9.05-9.30   : Team Discussion about work Progress
+10.40-12.30 : Layout Integration and corrections in Layout
+12.35-12.56 : Client(Rafi) Meeting
+2.00-2.20   : Uploading Layout pages as static pages to Git publish
+2.20-2.50   : Identify the Unique and Common Layout pages for Estimation
+3.00-4.00   : Web Api Session amoung Team
+4.30-4.50   : Presenting the Layout to the Client(Rafi)
+4.50-5.00   : Discussion with Layout team about changes in Layout
+5.00-5.40   : Discussion about Layout page Estimation</t>
+  </si>
+  <si>
+    <t>9.30-10.20  : Softskill session
+10.20-10.40 : Tea Break
+1.00-2.00   : Lunch Break
+4.00-4.30   : Tea Break</t>
+  </si>
+  <si>
     <t>Estimation and Layout Correction</t>
   </si>
   <si>
@@ -1600,30 +1628,336 @@
     <t>Refining the layout and responvise</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimation explanation meeting-15 min
-30mins : Helping in Attendence Layout
-15 mins : meeting with Rafi 
-1.30 mins : Estimation
-10 mins : Layout Correction Explanation
+    <t xml:space="preserve">8.45-9.05 : Updating Timesheet 
+9:05 - 9:30 : Team meeting
+12:35 - 12:56 : meeting with Rafi 
+2.00-3.00 : Identifying the Unique page for Estimation
+4.35-4.50 : Web API Session with team 
+4.55-5.30: Layout Correction Explanation and Estimation
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Softskill-1 hour
-webAPI Session with team-1 hour, Prepare for Review -100 mins
-lunch and Break-80 mins </t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>9:30 - 10:20 - Softskill session</t>
+    <t xml:space="preserve">
+9.30-10.20 : Soft skill
+10.30-11.45: prepare for internal review
+1-1.45-Lunch
+4.35-4.50 : Web API Session with other team 
+5.30-6: Internal Review with Anitha
+</t>
+  </si>
+  <si>
+    <t>Layout page for Assign course and Create topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:20-9:30-Team meeting,
+10:40-12:30:Worked on Layout page (Assign course and create topic),
+12:35-12:55:Meeting with Rafi,
+2:00-3:00: Web Api session among team,
+4:30-5:30-Layout corrections and responsivenss 
+</t>
+  </si>
+  <si>
+    <t>9:30-10:20:Softskill session,
+10:20-10:40:Break,
+1:00-1:50:lunch break,
+3:00-4:00:Explored about entity framework,
+4:00-4:20:Tea break,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet 
+9:05 - 9:30 : Team meeting
+9:30 - 10:20 : Softskill session(Problem Solving)
+10:20 - 10:40 : break
+10:40-10:55 : Estimation explanation meeting
+11.00-12.30: worked on attendace layout
+12:35 - 12:56 : meeting with Rafi 
+1:00 - 1:40 : Lunch
+2:00 - 3:00: webAPI Session with team members
+3.00-3.40:exploration on html
+3.40-4.00:uploading code in github
+4:30- 4:45 : break
+4.45-5.45:Exploration on web api
+7.00-8.00:Brushing up of basic concepts in c#
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     3 Hrs and 40 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                              5 hrs and 10 mins</t>
+  </si>
+  <si>
+    <t>creating component in angular</t>
+  </si>
+  <si>
+    <t>8:50-9:00   : Updating Timesheet
+9:05-9:30   : Team Discussion about work Progress
+10:40-12:30 : intergarting the layout (TMS layout)
+12:35-12:56 : Client(Rafi) Meeting
+2:00-2:20   : creating the repositories and uploading the static page in github
+2:20-2:50   :  spliting the common page and prepaing for estimation
+3:00-4:00   : Web Api Session amoung Team
+4:30-4:50   : Presenting the Layout to the Client(Rafi)
+4:50-5:00   : Discussion with Layout team about changes in Layout
+5:00-5:40   : Discussion about Layout page Estimation               7:00-7:30   : correcting the changes in the layout</t>
+  </si>
+  <si>
+    <t>9:30-10:20  : Softskill session
+10:20-10:40 : Tea Break
+1:00-2:00   : Lunch Break
+4:00-4:30   : Tea Break</t>
+  </si>
+  <si>
+    <t>Exploration on web api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00    : Updating Timesheet
+9:00 - 9:30  : Team meeting
+10:40-10:55  : Estimation explanation meeting
+11:00-11:45  : Refining Feedback layout, intergrating with other layouts and updating in git 
+11.45-12.15  : Helping in Estimation
+12:35 - 12:56: meeting with Rafi 
+2.00-3.00    : Identifying the pages and Estimation
+3.00-4.00    : Web API Session with team 
+4.30-4.50    : Web API Session with other team 
+4.55- 5.45   : Exploring web api and installing packages ,Estimationing layout pages
+</t>
+  </si>
+  <si>
+    <t>9:30 - 10:20 : Softskill
+10.20 -10.40 : Break
+1.00-1.40    : Lunch</t>
+  </si>
+  <si>
+    <t>Estimation for TMS and refineed layouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.45-9.00 : Updating Timesheet and HLD Document
+9:05 - 9:30 : Team meeting for work status
+10:40-10:55 : Estimation explanation meeting with team
+11:00-11:45 : Refining schedule review and review layout for TMS 
+11:45-12:30 : reviewing others layouts
+12:35 - 12:56 : meeting with client 
+2:00-3:00 : Identifying the pages for Estimation
+4.55-5.45: Layout Correction Explanation and Estimation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:30 - 10:20 : Softskill session
+10:20 - 10:40 : break
+1:00 - 1:40 : Lunch break
+3:00 - 4:00: Web API Session with team members
+4:00- 4:20 : break
+4.35-4.50 : Entity framework Session with other team </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource </t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Task Type</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Timesheet and MOM updating</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting </t>
+  </si>
+  <si>
+    <t>Non Project</t>
+  </si>
+  <si>
+    <t>Api Service refining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration </t>
+  </si>
+  <si>
+    <t>Customer Meeting</t>
+  </si>
+  <si>
+    <t>Customer Review</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;Typescript Intorduction and Sample programs&gt;</t>
+  </si>
+  <si>
+    <t>Api Service implementation on Controller</t>
+  </si>
+  <si>
+    <t>Lunch and Break</t>
+  </si>
+  <si>
+    <t>Service explanation to Members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunch </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Morning Break</t>
+  </si>
+  <si>
+    <t>Evening Break</t>
+  </si>
+  <si>
+    <t>Api Swagger Testing</t>
+  </si>
+  <si>
+    <t>Soft Skill</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;Topics&gt;</t>
+  </si>
+  <si>
+    <t>Working on HTML layout</t>
+  </si>
+  <si>
+    <t>Time Sheet</t>
+  </si>
+  <si>
+    <t>Database Migration</t>
+  </si>
+  <si>
+    <t>Logging in user services &amp; user controller</t>
+  </si>
+  <si>
+    <t>User Services List of Users by Role</t>
+  </si>
+  <si>
+    <t>client meeting</t>
+  </si>
+  <si>
+    <t>helping other team with ui</t>
+  </si>
+  <si>
+    <t>fixing errors in user services</t>
+  </si>
+  <si>
+    <t>ef core exploration</t>
+  </si>
+  <si>
+    <t>CRUD Operation in user Services</t>
+  </si>
+  <si>
+    <t>Technical Session</t>
+  </si>
+  <si>
+    <t>Time Sheet Updating</t>
+  </si>
+  <si>
+    <t>Estimation for Dashboard</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;Typescript Introduction and  Installation&gt;</t>
+  </si>
+  <si>
+    <t>Discussion about Services with Arul and Spliting Services</t>
+  </si>
+  <si>
+    <t>Service-Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating TimeSheet </t>
+  </si>
+  <si>
+    <t>Estimation Preparation</t>
+  </si>
+  <si>
+    <t>Web API Exploration (user services) with gokul</t>
+  </si>
+  <si>
+    <t>Working on Feedback services</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;TypeScript Introduction and Simple Examples&gt;</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;Introduction of Typescript , VS code Installation&gt;</t>
+  </si>
+  <si>
+    <t>Service Discussion with Arul and Spliting the Service</t>
+  </si>
+  <si>
+    <t>Service-Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepared for Internal Review </t>
+  </si>
+  <si>
+    <t>Working on WebAPI (Review )</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;data type &gt;</t>
+  </si>
+  <si>
+    <t>Timesheet Updating</t>
+  </si>
+  <si>
+    <t>Estimation for ProfileView</t>
+  </si>
+  <si>
+    <t>Learned Angular &lt;Typescript introduction&gt;</t>
+  </si>
+  <si>
+    <t>discussion on services and spliting the services</t>
+  </si>
+  <si>
+    <t>Service-Role</t>
+  </si>
+  <si>
+    <t>Estimation for unique pages</t>
+  </si>
+  <si>
+    <t>Timesheet</t>
+  </si>
+  <si>
+    <t>Working on HTML layout (Refining)</t>
+  </si>
+  <si>
+    <t>Estimation for department page</t>
+  </si>
+  <si>
+    <t>Pulling from git and Web API exploration</t>
+  </si>
+  <si>
+    <t>013:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-14009]hh:mm:ss;@"/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1767,13 +2101,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -1887,7 +2235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2038,6 +2386,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2065,80 +2492,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="21" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3348,14 +3842,14 @@
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="16" t="s">
@@ -3859,14 +4353,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="88" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
     </row>
     <row r="4" spans="1:22" ht="101.25" customHeight="1">
       <c r="A4" s="16" t="s">
@@ -4109,14 +4603,14 @@
       <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="88" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
     </row>
     <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="16" t="s">
@@ -4226,27 +4720,27 @@
       <c r="A10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="91" t="s">
         <v>298</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="93"/>
     </row>
     <row r="11" spans="1:7" ht="36.75" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="91" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="62"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="93"/>
     </row>
     <row r="12" spans="1:7" ht="84" customHeight="1">
       <c r="A12" s="16" t="s">
@@ -4279,8 +4773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14287F61-8AE3-4555-BA8D-07210E8D9156}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:G12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4524,238 +5018,3739 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7172FC-5606-4FD6-B7B3-02AB5BD496A0}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25" style="65"/>
-    <col min="2" max="2" width="30.28515625" style="65" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" style="65" customWidth="1"/>
-    <col min="4" max="4" width="25" style="65"/>
-    <col min="5" max="5" width="47" style="65" customWidth="1"/>
-    <col min="6" max="6" width="42" style="65" customWidth="1"/>
-    <col min="7" max="16384" width="25" style="65"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="66" t="s">
+      <c r="F1" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="69" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="267" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="58" t="s">
         <v>464</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="58" t="s">
         <v>465</v>
       </c>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>466</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="58" t="s">
         <v>467</v>
       </c>
-      <c r="G2" s="82"/>
-    </row>
-    <row r="3" spans="1:7" ht="89.25">
-      <c r="A3" s="67" t="s">
+      <c r="G2" s="70"/>
+    </row>
+    <row r="3" spans="1:7" ht="147.75" customHeight="1">
+      <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="68" t="s">
-        <v>346</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69" t="s">
+      <c r="B3" s="58" t="s">
         <v>468</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59" t="s">
         <v>469</v>
       </c>
-      <c r="G3" s="83"/>
+      <c r="F3" s="59" t="s">
+        <v>470</v>
+      </c>
+      <c r="G3" s="71"/>
     </row>
     <row r="4" spans="1:7" ht="244.5" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="70" t="s">
-        <v>470</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="B4" s="60" t="s">
         <v>471</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71" t="s">
+      <c r="C4" s="60" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="G4" s="64"/>
-    </row>
-    <row r="5" spans="1:7" ht="133.5" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:7" ht="228.75" customHeight="1">
+      <c r="A5" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="62" t="s">
+        <v>473</v>
+      </c>
+      <c r="C5" s="58" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="68" t="s">
-        <v>440</v>
-      </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68" t="s">
-        <v>441</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>442</v>
-      </c>
-      <c r="G5" s="63"/>
-    </row>
-    <row r="6" spans="1:7" ht="150" customHeight="1">
-      <c r="A6" s="67" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="58" t="s">
+        <v>474</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>475</v>
+      </c>
+      <c r="G5" s="54"/>
+    </row>
+    <row r="6" spans="1:7" ht="120" customHeight="1">
+      <c r="A6" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="74"/>
-      <c r="C6" s="68" t="s">
-        <v>472</v>
-      </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="75" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="58" t="s">
+        <v>476</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="64" t="s">
+        <v>477</v>
+      </c>
+      <c r="F6" s="64" t="s">
+        <v>478</v>
+      </c>
+      <c r="G6" s="72"/>
+    </row>
+    <row r="7" spans="1:7" ht="162" customHeight="1">
+      <c r="A7" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>473</v>
       </c>
-      <c r="F6" s="75" t="s">
-        <v>474</v>
-      </c>
-      <c r="G6" s="84"/>
-    </row>
-    <row r="7" spans="1:7" ht="132.75" customHeight="1">
-      <c r="A7" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68" t="s">
-        <v>475</v>
-      </c>
-      <c r="D7" s="68"/>
-      <c r="E7" s="75" t="s">
-        <v>476</v>
-      </c>
-      <c r="F7" s="86" t="s">
-        <v>477</v>
-      </c>
-      <c r="G7" s="82"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="67" t="s">
+      <c r="C7" s="58" t="s">
+        <v>479</v>
+      </c>
+      <c r="D7" s="58"/>
+      <c r="E7" s="64" t="s">
+        <v>480</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>481</v>
+      </c>
+      <c r="G7" s="70"/>
+    </row>
+    <row r="8" spans="1:7" ht="150" customHeight="1">
+      <c r="A8" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69" t="s">
-        <v>478</v>
-      </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="82"/>
-    </row>
-    <row r="9" spans="1:7" ht="63.75">
-      <c r="A9" s="67" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="74" t="s">
+        <v>482</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59" t="s">
+        <v>483</v>
+      </c>
+      <c r="F8" s="65" t="s">
+        <v>484</v>
+      </c>
+      <c r="G8" s="70"/>
+    </row>
+    <row r="9" spans="1:7" ht="230.25" customHeight="1">
+      <c r="A9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="58" t="s">
         <v>302</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>454</v>
-      </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="75" t="s">
-        <v>455</v>
-      </c>
-      <c r="F9" s="69" t="s">
-        <v>429</v>
-      </c>
-      <c r="G9" s="82"/>
-    </row>
-    <row r="10" spans="1:7" ht="75.75" customHeight="1">
-      <c r="A10" s="67" t="s">
+      <c r="C9" s="58" t="s">
+        <v>485</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="64" t="s">
+        <v>486</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>487</v>
+      </c>
+      <c r="G9" s="70"/>
+    </row>
+    <row r="10" spans="1:7" ht="204.75" customHeight="1">
+      <c r="A10" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68" t="s">
-        <v>430</v>
-      </c>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68" t="s">
-        <v>431</v>
-      </c>
-      <c r="F10" s="68" t="s">
-        <v>374</v>
-      </c>
-      <c r="G10" s="82"/>
-    </row>
-    <row r="11" spans="1:7" ht="144" customHeight="1">
-      <c r="A11" s="67" t="s">
+      <c r="B10" s="58" t="s">
+        <v>488</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>319</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58" t="s">
+        <v>489</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>490</v>
+      </c>
+      <c r="G10" s="70"/>
+    </row>
+    <row r="11" spans="1:7" ht="189.75" customHeight="1">
+      <c r="A11" s="57" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>456</v>
-      </c>
-      <c r="C11" s="80" t="s">
-        <v>457</v>
-      </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="75" t="s">
-        <v>473</v>
-      </c>
-      <c r="F11" s="75" t="s">
-        <v>459</v>
+        <v>491</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="64" t="s">
+        <v>492</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="141.75" customHeight="1">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="79" t="s">
-        <v>461</v>
-      </c>
-      <c r="F12" s="69" t="s">
-        <v>479</v>
-      </c>
-      <c r="G12" s="85"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67" t="s">
+        <v>494</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="68" t="s">
+        <v>495</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>496</v>
+      </c>
+      <c r="G12" s="73"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:G12">
     <sortCondition ref="A2:A12"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C319A4C-EADA-4641-96D7-D7B692B906C8}">
+  <dimension ref="A1:Q165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="84" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="84" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="84" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="78" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="78" t="s">
+        <v>498</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>500</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>501</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>502</v>
+      </c>
+      <c r="G1" s="82"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D2" s="81">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E2" s="81">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="F2" s="81">
+        <f>E2-D2</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="H2" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I2" s="79" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="94"/>
+      <c r="B3" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D3" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E3" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F3" s="81">
+        <f t="shared" ref="F3:F60" si="0">E3-D3</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I3" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H3)</f>
+        <v>0.14583333333333331</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="94"/>
+      <c r="B4" s="80" t="s">
+        <v>510</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D4" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E4" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F4" s="81">
+        <f>E4-D4</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="H4" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I4" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H4)</f>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="94"/>
+      <c r="B5" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D5" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E5" s="81">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F5" s="81">
+        <f>E5-D5</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="H5" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I5" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H5)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="94"/>
+      <c r="B6" s="80" t="s">
+        <v>514</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D6" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E6" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F6" s="81">
+        <f>E6-D6</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H6" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I6" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H6)</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="94"/>
+      <c r="B7" s="80" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D7" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E7" s="81">
+        <v>0.6875</v>
+      </c>
+      <c r="F7" s="81">
+        <f>E7-D7</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="H7" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I7" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H7)</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="94"/>
+      <c r="B8" s="80" t="s">
+        <v>517</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D8" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E8" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F8" s="81">
+        <f>E8-D8</f>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="H8" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I8" s="81">
+        <f>SUMIFS(F2:F16, C2:C16,H8)</f>
+        <v>3.819444444444442E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="94"/>
+      <c r="B9" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C9" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D9" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E9" s="81">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F9" s="81">
+        <f>E9-D9</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="H9" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I9" s="79">
+        <f>SUM(I3:I8)</f>
+        <v>0.35763888888888873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="94"/>
+      <c r="B10" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D10" s="81">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E10" s="81">
+        <v>0.4375</v>
+      </c>
+      <c r="F10" s="81">
+        <f>E10-D10</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="I10" s="84"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="94"/>
+      <c r="B11" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D11" s="81">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E11" s="81">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="F11" s="81">
+        <f>E11-D11</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="I11" s="84"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="94"/>
+      <c r="B12" s="80" t="s">
+        <v>522</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D12" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E12" s="81">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="F12" s="81">
+        <f>E12-D12</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="94"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81">
+        <f>E13-D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="94"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81">
+        <f>E14-D14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="94"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="94"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+      <c r="F16" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C17" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D17" s="81">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E17" s="81">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F17" s="81">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="H17" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I17" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="94"/>
+      <c r="B18" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D18" s="81">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E18" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F18" s="81">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H18" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I18" s="81">
+        <f t="shared" ref="I18" si="1">SUMIFS(F17:F31, C17:C31,H18)</f>
+        <v>0.22916666666666674</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="94"/>
+      <c r="B19" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C19" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D19" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E19" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F19" s="81">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="H19" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I19" s="81">
+        <f t="shared" ref="I19" si="2">SUMIFS(F17:F31, C17:C31,H19)</f>
+        <v>7.2916666666666685E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="94"/>
+      <c r="B20" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C20" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D20" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E20" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F20" s="81">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="H20" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I20" s="81">
+        <f t="shared" ref="I20" si="3">SUMIFS(F17:F31, C17:C31,H20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="94"/>
+      <c r="B21" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C21" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D21" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E21" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F21" s="81">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="H21" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I21" s="81">
+        <f t="shared" ref="I21" si="4">SUMIFS(F17:F31, C17:C31,H21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="94"/>
+      <c r="B22" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C22" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D22" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E22" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F22" s="81">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="H22" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I22" s="81">
+        <f t="shared" ref="I22" si="5">SUMIFS(F17:F31, C17:C31,H22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="94"/>
+      <c r="B23" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C23" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D23" s="81">
+        <v>0.65625</v>
+      </c>
+      <c r="E23" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F23" s="81">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="H23" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I23" s="81">
+        <f t="shared" ref="I23" si="6">SUMIFS(F17:F31, C17:C31,H23)</f>
+        <v>3.8194444444444309E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="94"/>
+      <c r="B24" s="80" t="s">
+        <v>524</v>
+      </c>
+      <c r="C24" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D24" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E24" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="F24" s="81">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="H24" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I24" s="79">
+        <f t="shared" ref="I24" si="7">SUM(I18:I23)</f>
+        <v>0.34027777777777773</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="94"/>
+      <c r="B25" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="C25" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D25" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="E25" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="F25" s="81">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="I25" s="84"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="94"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="84"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="94"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="94"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="94"/>
+      <c r="B29" s="80"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="94"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="94"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="94" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="80" t="s">
+        <v>526</v>
+      </c>
+      <c r="C32" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D32" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E32" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F32" s="81">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I32" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="94"/>
+      <c r="B33" s="80" t="s">
+        <v>527</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D33" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E33" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F33" s="81">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H33" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I33" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H33)</f>
+        <v>0.12847222222222221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="94"/>
+      <c r="B34" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C34" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D34" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E34" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F34" s="81">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I34" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H34)</f>
+        <v>2.3611111111111083E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="94"/>
+      <c r="B35" s="80" t="s">
+        <v>528</v>
+      </c>
+      <c r="C35" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D35" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E35" s="81">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F35" s="81">
+        <f t="shared" si="0"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="H35" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I35" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H35)</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="94"/>
+      <c r="B36" s="80" t="s">
+        <v>529</v>
+      </c>
+      <c r="C36" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D36" s="81">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E36" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F36" s="81">
+        <f>E36-D36</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H36" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I36" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H36)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="94"/>
+      <c r="B37" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C37" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D37" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E37" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F37" s="81">
+        <f>E37-D37</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H37" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I37" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H37)</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="94"/>
+      <c r="B38" s="80" t="s">
+        <v>530</v>
+      </c>
+      <c r="C38" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D38" s="81">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E38" s="81">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F38" s="81">
+        <f>E38-D38</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="H38" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I38" s="81">
+        <f>SUMIFS(F32:F45, C32:C45,H38)</f>
+        <v>4.9999999999999933E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="94"/>
+      <c r="B39" s="80" t="s">
+        <v>531</v>
+      </c>
+      <c r="C39" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D39" s="81">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="E39" s="81">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="F39" s="81">
+        <f>E39-D39</f>
+        <v>9.7222222222221877E-3</v>
+      </c>
+      <c r="H39" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I39" s="79">
+        <f t="shared" ref="I39" si="8">SUM(I33:I38)</f>
+        <v>0.35069444444444436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="94"/>
+      <c r="B40" s="80" t="s">
+        <v>532</v>
+      </c>
+      <c r="C40" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D40" s="81">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E40" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F40" s="81">
+        <f>E40-D40</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="I40" s="84"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="94"/>
+      <c r="B41" s="80" t="s">
+        <v>533</v>
+      </c>
+      <c r="C41" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D41" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E41" s="81">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F41" s="81">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K41" s="81"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="94"/>
+      <c r="B42" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C42" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D42" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E42" s="81">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="F42" s="81">
+        <f t="shared" si="0"/>
+        <v>3.2638888888888884E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="94"/>
+      <c r="B43" s="80" t="s">
+        <v>534</v>
+      </c>
+      <c r="C43" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D43" s="81">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="E43" s="81">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F43" s="81">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="94"/>
+      <c r="B44" s="80" t="s">
+        <v>535</v>
+      </c>
+      <c r="C44" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D44" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E44" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F44" s="81">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="94"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="94" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="80" t="s">
+        <v>536</v>
+      </c>
+      <c r="C46" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D46" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E46" s="81">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F46" s="81">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="H46" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I46" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="94"/>
+      <c r="B47" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C47" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D47" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E47" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F47" s="81">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H47" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I47" s="81">
+        <f t="shared" ref="I47" si="9">SUMIFS(F46:F60, C46:C60,H47)</f>
+        <v>0.14236111111111099</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="94"/>
+      <c r="B48" s="80" t="s">
+        <v>537</v>
+      </c>
+      <c r="C48" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D48" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E48" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F48" s="81">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H48" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I48" s="81">
+        <f t="shared" ref="I48" si="10">SUMIFS(F46:F60, C46:C60,H48)</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="94"/>
+      <c r="B49" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C49" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D49" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E49" s="81">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F49" s="81">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="H49" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I49" s="81">
+        <f t="shared" ref="I49" si="11">SUMIFS(F46:F60, C46:C60,H49)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="94"/>
+      <c r="B50" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C50" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D50" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E50" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F50" s="81">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="H50" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I50" s="81">
+        <f t="shared" ref="I50" si="12">SUMIFS(F46:F60, C46:C60,H50)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="94"/>
+      <c r="B51" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C51" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D51" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E51" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F51" s="81">
+        <f t="shared" si="0"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H51" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I51" s="81">
+        <f t="shared" ref="I51" si="13">SUMIFS(F46:F60, C46:C60,H51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="94"/>
+      <c r="B52" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C52" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D52" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E52" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F52" s="81">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="H52" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I52" s="81">
+        <f t="shared" ref="I52" si="14">SUMIFS(F46:F60, C46:C60,H52)</f>
+        <v>6.9444444444444531E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="94"/>
+      <c r="B53" s="80" t="s">
+        <v>538</v>
+      </c>
+      <c r="C53" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D53" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E53" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F53" s="81">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H53" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I53" s="79">
+        <f t="shared" ref="I53" si="15">SUM(I47:I52)</f>
+        <v>0.32638888888888884</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="94"/>
+      <c r="B54" s="80" t="s">
+        <v>539</v>
+      </c>
+      <c r="C54" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D54" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E54" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F54" s="81">
+        <f t="shared" si="0"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="I54" s="84"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="94"/>
+      <c r="B55" s="80" t="s">
+        <v>540</v>
+      </c>
+      <c r="C55" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D55" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="E55" s="81">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F55" s="81">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="I55" s="84"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="94"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="94"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
+      <c r="F57" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="94"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
+      <c r="F58" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="94"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+      <c r="F59" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="94"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="81"/>
+      <c r="E60" s="81"/>
+      <c r="F60" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="80" t="s">
+        <v>541</v>
+      </c>
+      <c r="C61" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D61" s="81">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E61" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="F61" s="81">
+        <f>E61-D61</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="H61" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I61" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="94"/>
+      <c r="B62" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="C62" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D62" s="81">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E62" s="81">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="F62" s="81">
+        <f>E62-D62</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="H62" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I62" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H62)</f>
+        <v>0.10069444444444438</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="94"/>
+      <c r="B63" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C63" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D63" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E63" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F63" s="81">
+        <f>E63-D63</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H63" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I63" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H63)</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="94"/>
+      <c r="B64" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C64" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D64" s="81">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E64" s="81">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="F64" s="81">
+        <f>E64-D64</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="H64" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I64" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H64)</f>
+        <v>3.0625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="94"/>
+      <c r="B65" s="80" t="s">
+        <v>542</v>
+      </c>
+      <c r="C65" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D65" s="81">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="E65" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F65" s="81">
+        <f>E65-D65</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="H65" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I65" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H65)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="94"/>
+      <c r="B66" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C66" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D66" s="81">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E66" s="81">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F66" s="81">
+        <f>E66-D66</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="H66" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I66" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H66)</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="94"/>
+      <c r="B67" s="80" t="s">
+        <v>543</v>
+      </c>
+      <c r="C67" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D67" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E67" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F67" s="81">
+        <f>E67-D67</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="H67" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I67" s="81">
+        <f>SUMIFS(F61:F71, C61:C71,H67)</f>
+        <v>6.2500000000000167E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="94"/>
+      <c r="B68" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C68" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D68" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E68" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F68" s="81">
+        <f>E68-D68</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="H68" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I68" s="79">
+        <f t="shared" ref="I68" si="16">SUM(I62:I67)</f>
+        <v>3.3013888888888889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="94"/>
+      <c r="B69" s="80" t="s">
+        <v>544</v>
+      </c>
+      <c r="C69" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D69" s="81">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="E69" s="81">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F69" s="81">
+        <f>E69-D69</f>
+        <v>4.8611111111111119E-2</v>
+      </c>
+      <c r="I69" s="84"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="94"/>
+      <c r="B70" s="80" t="s">
+        <v>545</v>
+      </c>
+      <c r="C70" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D70" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E70" s="81">
+        <v>3.7083333333333335</v>
+      </c>
+      <c r="F70" s="81">
+        <f>E70-D70</f>
+        <v>3.0625</v>
+      </c>
+      <c r="I70" s="84"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="94"/>
+      <c r="B71" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C71" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D71" s="81">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="E71" s="81">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="F71" s="81">
+        <f>E71-D71</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="94"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="94"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="94"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="94"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="94" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C76" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D76" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E76" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F76" s="81">
+        <f t="shared" ref="F76:F129" si="17">E76-D76</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H76" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I76" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="94"/>
+      <c r="B77" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C77" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D77" s="81">
+        <v>0</v>
+      </c>
+      <c r="E77" s="81">
+        <v>0</v>
+      </c>
+      <c r="F77" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H77" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I77" s="81">
+        <f t="shared" ref="I77" si="18">SUMIFS(F76:F90, C76:C90,H77)</f>
+        <v>0.12986111111111098</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="94"/>
+      <c r="B78" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C78" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D78" s="81">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E78" s="81">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F78" s="81">
+        <f t="shared" si="17"/>
+        <v>2.5694444444444353E-2</v>
+      </c>
+      <c r="H78" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I78" s="81">
+        <f t="shared" ref="I78" si="19">SUMIFS(F76:F90, C76:C90,H78)</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="94"/>
+      <c r="B79" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C79" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D79" s="81">
+        <v>0</v>
+      </c>
+      <c r="E79" s="81">
+        <v>0</v>
+      </c>
+      <c r="F79" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H79" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I79" s="81">
+        <f t="shared" ref="I79" si="20">SUMIFS(F76:F90, C76:C90,H79)</f>
+        <v>6.3888888888888884E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="94"/>
+      <c r="B80" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C80" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D80" s="81">
+        <v>0.53125</v>
+      </c>
+      <c r="E80" s="81">
+        <v>0.5625</v>
+      </c>
+      <c r="F80" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H80" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I80" s="81">
+        <f t="shared" ref="I80" si="21">SUMIFS(F76:F90, C76:C90,H80)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="94"/>
+      <c r="B81" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C81" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D81" s="81">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E81" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F81" s="81">
+        <f t="shared" si="17"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H81" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I81" s="81">
+        <f t="shared" ref="I81" si="22">SUMIFS(F76:F90, C76:C90,H81)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="94"/>
+      <c r="B82" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C82" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D82" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E82" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F82" s="81">
+        <f t="shared" si="17"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="H82" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I82" s="81">
+        <f t="shared" ref="I82" si="23">SUMIFS(F76:F90, C76:C90,H82)</f>
+        <v>5.5555555555555636E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="94"/>
+      <c r="B83" s="80" t="s">
+        <v>546</v>
+      </c>
+      <c r="C83" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D83" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E83" s="81">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="F83" s="81">
+        <f t="shared" si="17"/>
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="H83" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I83" s="79">
+        <f t="shared" ref="I83" si="24">SUM(I77:I82)</f>
+        <v>0.29444444444444434</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="94"/>
+      <c r="B84" s="80" t="s">
+        <v>526</v>
+      </c>
+      <c r="C84" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D84" s="81">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E84" s="81">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="F84" s="81">
+        <f t="shared" si="17"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="I84" s="84"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="94"/>
+      <c r="B85" s="80" t="s">
+        <v>547</v>
+      </c>
+      <c r="C85" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D85" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E85" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F85" s="81">
+        <f>E85-D85</f>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="I85" s="84"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="94"/>
+      <c r="B86" s="80" t="s">
+        <v>548</v>
+      </c>
+      <c r="C86" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D86" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="E86" s="81">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="F86" s="81">
+        <f t="shared" si="17"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="94"/>
+      <c r="B87" s="80"/>
+      <c r="C87" s="80"/>
+      <c r="D87" s="81"/>
+      <c r="E87" s="81"/>
+      <c r="F87" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="94"/>
+      <c r="B88" s="80"/>
+      <c r="C88" s="80"/>
+      <c r="D88" s="81"/>
+      <c r="E88" s="81"/>
+      <c r="F88" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="94"/>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
+      <c r="F89" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="94"/>
+      <c r="B90" s="80"/>
+      <c r="C90" s="80"/>
+      <c r="D90" s="81"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C91" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D91" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E91" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F91" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H91" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I91" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="94"/>
+      <c r="B92" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C92" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D92" s="81">
+        <v>0</v>
+      </c>
+      <c r="E92" s="81">
+        <v>0</v>
+      </c>
+      <c r="F92" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H92" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I92" s="81">
+        <f t="shared" ref="I92" si="25">SUMIFS(F91:F105, C91:C105,H92)</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="94"/>
+      <c r="B93" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C93" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D93" s="81">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E93" s="81">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F93" s="81">
+        <f t="shared" si="17"/>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="H93" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I93" s="81">
+        <f t="shared" ref="I93" si="26">SUMIFS(F91:F105, C91:C105,H93)</f>
+        <v>0.16666666666666663</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="94"/>
+      <c r="B94" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C94" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D94" s="81">
+        <v>0</v>
+      </c>
+      <c r="E94" s="81">
+        <v>0</v>
+      </c>
+      <c r="F94" s="81">
+        <f>E94-D94</f>
+        <v>0</v>
+      </c>
+      <c r="H94" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I94" s="81">
+        <f t="shared" ref="I94" si="27">SUMIFS(F91:F105, C91:C105,H94)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="94"/>
+      <c r="B95" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C95" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D95" s="81">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E95" s="81">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="F95" s="81">
+        <f t="shared" si="17"/>
+        <v>2.7777777777777901E-2</v>
+      </c>
+      <c r="H95" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I95" s="81">
+        <f t="shared" ref="I95" si="28">SUMIFS(F91:F105, C91:C105,H95)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="94"/>
+      <c r="B96" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C96" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D96" s="81">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="E96" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F96" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H96" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I96" s="81">
+        <f t="shared" ref="I96" si="29">SUMIFS(F91:F105, C91:C105,H96)</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="94"/>
+      <c r="B97" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C97" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D97" s="81">
+        <v>0.65625</v>
+      </c>
+      <c r="E97" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F97" s="81">
+        <f t="shared" si="17"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="H97" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I97" s="81">
+        <f t="shared" ref="I97" si="30">SUMIFS(F91:F105, C91:C105,H97)</f>
+        <v>6.9444444444444531E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="94"/>
+      <c r="B98" s="80" t="s">
+        <v>549</v>
+      </c>
+      <c r="C98" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D98" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E98" s="81">
+        <v>0.6875</v>
+      </c>
+      <c r="F98" s="81">
+        <f t="shared" si="17"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="H98" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I98" s="79">
+        <f t="shared" ref="I98" si="31">SUM(I92:I97)</f>
+        <v>0.30486111111111119</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="94"/>
+      <c r="B99" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="C99" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D99" s="81">
+        <v>0</v>
+      </c>
+      <c r="E99" s="81">
+        <v>0</v>
+      </c>
+      <c r="F99" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="I99" s="84"/>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="94"/>
+      <c r="B100" s="80" t="s">
+        <v>541</v>
+      </c>
+      <c r="C100" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D100" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E100" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F100" s="81">
+        <f t="shared" si="17"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="I100" s="84"/>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="94"/>
+      <c r="B101" s="80" t="s">
+        <v>535</v>
+      </c>
+      <c r="C101" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D101" s="81">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E101" s="81">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F101" s="81">
+        <f t="shared" si="17"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="94"/>
+      <c r="B102" s="80"/>
+      <c r="C102" s="80"/>
+      <c r="D102" s="81"/>
+      <c r="E102" s="81"/>
+      <c r="F102" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="94"/>
+      <c r="B103" s="80"/>
+      <c r="C103" s="80"/>
+      <c r="D103" s="81"/>
+      <c r="E103" s="81"/>
+      <c r="F103" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="94"/>
+      <c r="B104" s="80"/>
+      <c r="C104" s="80"/>
+      <c r="D104" s="81"/>
+      <c r="E104" s="81"/>
+      <c r="F104" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="94"/>
+      <c r="B105" s="80"/>
+      <c r="C105" s="80"/>
+      <c r="D105" s="81"/>
+      <c r="E105" s="81"/>
+      <c r="F105" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C106" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D106" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E106" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F106" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H106" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I106" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="94"/>
+      <c r="B107" s="18" t="s">
+        <v>520</v>
+      </c>
+      <c r="C107" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D107" s="95">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E107" s="81">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="F107" s="81">
+        <f t="shared" si="17"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="H107" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I107" s="81" t="e">
+        <f>SUMIFS(F106:F120, C106:C120,H107)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="94"/>
+      <c r="B108" s="80"/>
+      <c r="C108" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D108" s="81"/>
+      <c r="E108" s="81"/>
+      <c r="F108" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="H108" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I108" s="81">
+        <f t="shared" ref="I108" si="32">SUMIFS(F106:F120, C106:C120,H108)</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="94"/>
+      <c r="B109" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="C109" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D109" s="95">
+        <v>0.4916666666666667</v>
+      </c>
+      <c r="E109" s="81">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="F109" s="81">
+        <f t="shared" si="17"/>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="H109" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I109" s="81">
+        <f t="shared" ref="I109" si="33">SUMIFS(F106:F120, C106:C120,H109)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="94"/>
+      <c r="B110" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C110" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D110" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E110" s="81">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F110" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H110" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I110" s="81">
+        <f t="shared" ref="I110" si="34">SUMIFS(F106:F120, C106:C120,H110)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="94"/>
+      <c r="B111" s="18" t="s">
+        <v>550</v>
+      </c>
+      <c r="C111" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D111" s="81">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="E111" s="81">
+        <v>0.625</v>
+      </c>
+      <c r="F111" s="81">
+        <f t="shared" si="17"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="H111" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I111" s="81">
+        <f t="shared" ref="I111" si="35">SUMIFS(F106:F120, C106:C120,H111)</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="94"/>
+      <c r="B112" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C112" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D112" s="81">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="E112" s="81">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="F112" s="81">
+        <f t="shared" si="17"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="H112" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I112" s="81">
+        <f t="shared" ref="I112" si="36">SUMIFS(F106:F120, C106:C120,H112)</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" s="94"/>
+      <c r="B113" s="80" t="s">
+        <v>550</v>
+      </c>
+      <c r="C113" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D113" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E113" s="81">
+        <v>0.625</v>
+      </c>
+      <c r="F113" s="81" t="e">
+        <f>#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H113" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I113" s="79" t="e">
+        <f t="shared" ref="I113" si="37">SUM(I107:I112)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" s="94"/>
+      <c r="C114" s="80"/>
+      <c r="F114" s="81"/>
+      <c r="I114" s="84"/>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" s="94"/>
+      <c r="B115" s="80" t="s">
+        <v>541</v>
+      </c>
+      <c r="C115" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D115" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E115" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F115" s="81">
+        <f t="shared" si="17"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="I115" s="84"/>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" s="94"/>
+      <c r="B116" s="80" t="s">
+        <v>551</v>
+      </c>
+      <c r="C116" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D116" s="95">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E116" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F116" s="81">
+        <f t="shared" si="17"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" s="94"/>
+      <c r="B117" s="80"/>
+      <c r="C117" s="80"/>
+      <c r="D117" s="81"/>
+      <c r="E117" s="81"/>
+      <c r="F117" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" s="94"/>
+      <c r="B118" s="80"/>
+      <c r="C118" s="80"/>
+      <c r="D118" s="81"/>
+      <c r="E118" s="81"/>
+      <c r="F118" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" s="94"/>
+      <c r="B119" s="80"/>
+      <c r="C119" s="80"/>
+      <c r="D119" s="81"/>
+      <c r="E119" s="81"/>
+      <c r="F119" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" s="94"/>
+      <c r="B120" s="80"/>
+      <c r="C120" s="80"/>
+      <c r="D120" s="81"/>
+      <c r="E120" s="81"/>
+      <c r="F120" s="81">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" s="94" t="s">
+        <v>22</v>
+      </c>
+      <c r="B121" s="80" t="s">
+        <v>552</v>
+      </c>
+      <c r="C121" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D121" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E121" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F121" s="81">
+        <f t="shared" si="17"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H121" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I121" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" s="94"/>
+      <c r="B122" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="C122" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D122" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E122" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F122" s="81">
+        <f t="shared" si="17"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H122" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I122" s="81">
+        <f t="shared" ref="I122" si="38">SUMIFS(F121:F135, C121:C135,H122)</f>
+        <v>0.17013888888888867</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" s="94"/>
+      <c r="B123" s="80" t="s">
+        <v>553</v>
+      </c>
+      <c r="C123" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D123" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E123" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F123" s="81">
+        <f t="shared" si="17"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H123" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I123" s="81">
+        <f t="shared" ref="I123" si="39">SUMIFS(F121:F135, C121:C135,H123)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124" s="94"/>
+      <c r="B124" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C124" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D124" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E124" s="81">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F124" s="81">
+        <f t="shared" si="17"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="H124" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I124" s="81">
+        <f t="shared" ref="I124" si="40">SUMIFS(F121:F135, C121:C135,H124)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" s="94"/>
+      <c r="B125" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C125" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D125" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E125" s="81">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F125" s="81">
+        <f t="shared" si="17"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="H125" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I125" s="81">
+        <f t="shared" ref="I125" si="41">SUMIFS(F121:F135, C121:C135,H125)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" s="94"/>
+      <c r="B126" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C126" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D126" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E126" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F126" s="81">
+        <f t="shared" si="17"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H126" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I126" s="81">
+        <f t="shared" ref="I126" si="42">SUMIFS(F121:F135, C121:C135,H126)</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="94"/>
+      <c r="B127" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C127" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D127" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E127" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F127" s="81">
+        <f t="shared" si="17"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="H127" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I127" s="81">
+        <f t="shared" ref="I127" si="43">SUMIFS(F121:F135, C121:C135,H127)</f>
+        <v>5.555555555555558E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" s="94"/>
+      <c r="B128" s="80" t="s">
+        <v>554</v>
+      </c>
+      <c r="C128" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D128" s="81">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E128" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F128" s="81">
+        <f t="shared" si="17"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H128" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I128" s="79">
+        <f t="shared" ref="I128" si="44">SUM(I122:I127)</f>
+        <v>0.34722222222222199</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" s="94"/>
+      <c r="B129" s="80" t="s">
+        <v>555</v>
+      </c>
+      <c r="C129" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D129" s="81">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E129" s="81">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F129" s="81">
+        <f t="shared" si="17"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="I129" s="84"/>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" s="94"/>
+      <c r="B130" s="80" t="s">
+        <v>556</v>
+      </c>
+      <c r="C130" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D130" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="E130" s="81">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F130" s="81">
+        <f t="shared" ref="F130:F165" si="45">E130-D130</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="I130" s="84"/>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" s="94"/>
+      <c r="B131" s="80" t="s">
+        <v>557</v>
+      </c>
+      <c r="C131" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D131" s="81">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E131" s="81">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F131" s="81">
+        <f t="shared" si="45"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" s="94"/>
+      <c r="B132" s="80" t="s">
+        <v>543</v>
+      </c>
+      <c r="C132" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D132" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E132" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F132" s="81">
+        <f t="shared" si="45"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" s="94"/>
+      <c r="B133" s="80"/>
+      <c r="C133" s="80"/>
+      <c r="D133" s="81"/>
+      <c r="E133" s="81"/>
+      <c r="F133" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" s="94"/>
+      <c r="B134" s="80"/>
+      <c r="C134" s="80"/>
+      <c r="D134" s="81"/>
+      <c r="E134" s="81"/>
+      <c r="F134" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
+      <c r="A135" s="94"/>
+      <c r="B135" s="80"/>
+      <c r="C135" s="80"/>
+      <c r="D135" s="81"/>
+      <c r="E135" s="81"/>
+      <c r="F135" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="A136" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B136" s="80" t="s">
+        <v>558</v>
+      </c>
+      <c r="C136" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D136" s="81">
+        <v>0.375</v>
+      </c>
+      <c r="E136" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F136" s="81">
+        <f t="shared" si="45"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H136" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I136" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="A137" s="94"/>
+      <c r="B137" s="80" t="s">
+        <v>559</v>
+      </c>
+      <c r="C137" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D137" s="81">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E137" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F137" s="81">
+        <f t="shared" si="45"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H137" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I137" s="81">
+        <f t="shared" ref="I137" si="46">SUMIFS(F136:F150, C136:C150,H137)</f>
+        <v>0.26388888888888901</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="A138" s="94"/>
+      <c r="B138" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C138" s="80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D138" s="81">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="E138" s="81">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="F138" s="81">
+        <f t="shared" si="45"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H138" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I138" s="81">
+        <f t="shared" ref="I138" si="47">SUMIFS(F136:F150, C136:C150,H138)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="A139" s="94"/>
+      <c r="B139" s="80" t="s">
+        <v>560</v>
+      </c>
+      <c r="C139" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D139" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E139" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F139" s="81">
+        <f t="shared" si="45"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H139" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I139" s="81">
+        <f t="shared" ref="I139" si="48">SUMIFS(F136:F150, C136:C150,H139)</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" s="94"/>
+      <c r="B140" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="C140" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D140" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E140" s="81">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="F140" s="81">
+        <f t="shared" si="45"/>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="H140" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I140" s="81">
+        <f t="shared" ref="I140" si="49">SUMIFS(F136:F150, C136:C150,H140)</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="94"/>
+      <c r="B141" s="80" t="s">
+        <v>561</v>
+      </c>
+      <c r="C141" s="80" t="s">
+        <v>511</v>
+      </c>
+      <c r="D141" s="81">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E141" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F141" s="81">
+        <f t="shared" si="45"/>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H141" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I141" s="81">
+        <f t="shared" ref="I141" si="50">SUMIFS(F136:F150, C136:C150,H141)</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="A142" s="94"/>
+      <c r="B142" s="80"/>
+      <c r="C142" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D142" s="81">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E142" s="81">
+        <v>0.125</v>
+      </c>
+      <c r="F142" s="81">
+        <f>E142-D142</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="H142" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I142" s="81">
+        <f t="shared" ref="I142" si="51">SUMIFS(F136:F150, C136:C150,H142)</f>
+        <v>7.2916666666666685E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="A143" s="94"/>
+      <c r="B143" s="80" t="s">
+        <v>524</v>
+      </c>
+      <c r="C143" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D143" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E143" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="F143" s="81">
+        <f>E143-D143</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="H143" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I143" s="79">
+        <f t="shared" ref="I143" si="52">SUM(I137:I142)</f>
+        <v>0.40972222222222232</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9">
+      <c r="A144" s="94"/>
+      <c r="B144" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="C144" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D144" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="E144" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="F144" s="81">
+        <f>E144-D144</f>
+        <v>0.125</v>
+      </c>
+      <c r="I144" s="84"/>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="A145" s="94"/>
+      <c r="B145" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C145" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D145" s="81">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E145" s="81">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F145" s="81">
+        <f>E145-D145</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="I145" s="84"/>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" s="94"/>
+      <c r="B146" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C146" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D146" s="81">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E146" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F146" s="81">
+        <f>E146-D146</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" s="94"/>
+      <c r="B147" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C147" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D147" s="81">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E147" s="81">
+        <v>0.125</v>
+      </c>
+      <c r="F147" s="81">
+        <f>E147-D147</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="A148" s="94"/>
+      <c r="B148" s="80"/>
+      <c r="C148" s="80"/>
+      <c r="D148" s="81"/>
+      <c r="E148" s="81"/>
+      <c r="F148" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" s="94"/>
+      <c r="B149" s="80"/>
+      <c r="C149" s="80"/>
+      <c r="D149" s="81"/>
+      <c r="E149" s="81"/>
+      <c r="F149" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="94"/>
+      <c r="B150" s="80"/>
+      <c r="C150" s="80"/>
+      <c r="D150" s="81"/>
+      <c r="E150" s="81"/>
+      <c r="F150" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" s="94" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151" s="80" t="s">
+        <v>507</v>
+      </c>
+      <c r="C151" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D151" s="81">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E151" s="81">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F151" s="81">
+        <f t="shared" si="45"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="H151" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="I151" s="79" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" s="94"/>
+      <c r="B152" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C152" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D152" s="81">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E152" s="81">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F152" s="81">
+        <f t="shared" si="45"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H152" s="83" t="s">
+        <v>504</v>
+      </c>
+      <c r="I152" s="81">
+        <f t="shared" ref="I152" si="53">SUMIFS(F151:F165, C151:C165,H152)</f>
+        <v>0.23958333333333343</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153" s="94"/>
+      <c r="B153" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="C153" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D153" s="81">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E153" s="81">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="F153" s="81">
+        <f t="shared" si="45"/>
+        <v>2.4305555555555636E-2</v>
+      </c>
+      <c r="H153" s="83" t="s">
+        <v>509</v>
+      </c>
+      <c r="I153" s="81">
+        <f t="shared" ref="I153" si="54">SUMIFS(F151:F165, C151:C165,H153)</f>
+        <v>7.2916666666666685E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" s="94"/>
+      <c r="B154" s="80" t="s">
+        <v>523</v>
+      </c>
+      <c r="C154" s="80" t="s">
+        <v>509</v>
+      </c>
+      <c r="D154" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E154" s="81">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F154" s="81">
+        <f t="shared" si="45"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="H154" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="I154" s="81">
+        <f t="shared" ref="I154" si="55">SUMIFS(F151:F165, C151:C165,H154)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" s="94"/>
+      <c r="B155" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="C155" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D155" s="81" t="s">
+        <v>562</v>
+      </c>
+      <c r="E155" s="81">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F155" s="81" t="e">
+        <f t="shared" si="45"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H155" s="83" t="s">
+        <v>508</v>
+      </c>
+      <c r="I155" s="81">
+        <f t="shared" ref="I155" si="56">SUMIFS(F151:F165, C151:C165,H155)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" s="94"/>
+      <c r="B156" s="80" t="s">
+        <v>520</v>
+      </c>
+      <c r="C156" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D156" s="81">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E156" s="81">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F156" s="81">
+        <f t="shared" si="45"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="H156" s="83" t="s">
+        <v>513</v>
+      </c>
+      <c r="I156" s="81">
+        <f t="shared" ref="I156" si="57">SUMIFS(F151:F165, C151:C165,H156)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" s="94"/>
+      <c r="B157" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C157" s="80" t="s">
+        <v>516</v>
+      </c>
+      <c r="D157" s="81">
+        <v>0.65625</v>
+      </c>
+      <c r="E157" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F157" s="81">
+        <f t="shared" si="45"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="H157" s="83" t="s">
+        <v>516</v>
+      </c>
+      <c r="I157" s="81" t="e">
+        <f t="shared" ref="I157" si="58">SUMIFS(F151:F165, C151:C165,H157)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" s="94"/>
+      <c r="B158" s="80" t="s">
+        <v>524</v>
+      </c>
+      <c r="C158" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D158" s="81">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E158" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="F158" s="81">
+        <f t="shared" si="45"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="H158" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="I158" s="79" t="e">
+        <f t="shared" ref="I158" si="59">SUM(I152:I157)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" s="94"/>
+      <c r="B159" s="80" t="s">
+        <v>525</v>
+      </c>
+      <c r="C159" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="D159" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="E159" s="81">
+        <v>0.875</v>
+      </c>
+      <c r="F159" s="81">
+        <f t="shared" si="45"/>
+        <v>0.125</v>
+      </c>
+      <c r="I159" s="84"/>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160" s="94"/>
+      <c r="B160" s="80"/>
+      <c r="C160" s="80"/>
+      <c r="D160" s="81"/>
+      <c r="E160" s="81"/>
+      <c r="F160" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="I160" s="84"/>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="94"/>
+      <c r="B161" s="80"/>
+      <c r="C161" s="80"/>
+      <c r="D161" s="81"/>
+      <c r="E161" s="81"/>
+      <c r="F161" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="94"/>
+      <c r="B162" s="80"/>
+      <c r="C162" s="80"/>
+      <c r="D162" s="81"/>
+      <c r="E162" s="81"/>
+      <c r="F162" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="94"/>
+      <c r="B163" s="80"/>
+      <c r="C163" s="80"/>
+      <c r="D163" s="81"/>
+      <c r="E163" s="81"/>
+      <c r="F163" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="94"/>
+      <c r="B164" s="80"/>
+      <c r="C164" s="80"/>
+      <c r="D164" s="81"/>
+      <c r="E164" s="81"/>
+      <c r="F164" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="94"/>
+      <c r="B165" s="80"/>
+      <c r="C165" s="80"/>
+      <c r="D165" s="81"/>
+      <c r="E165" s="81"/>
+      <c r="F165" s="81">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A76:A90"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="A17:A31"/>
+    <mergeCell ref="A32:A45"/>
+    <mergeCell ref="A46:A60"/>
+    <mergeCell ref="A61:A75"/>
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="A106:A120"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A136:A150"/>
+    <mergeCell ref="A151:A165"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3 I18 I33 I47 I62 I77 I92 I107 I122 I137 I152">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
+      <formula>0.25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="lessThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I19 I34 I48 I63 I78 I93 I108 I123 I138 I153">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="greaterThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 I20 I35 I49 I64 I79 I94 I109 I124 I139 I154">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+      <formula>0.0833333333333333</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0.0833333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6 I21 I36 I50 I65 I80 I95 I110 I125 I140 I155">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7 I22 I37 I51 I66 I81 I96 I111 I126 I141 I156">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0.0416666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8 I23 I38 I52 I67 I82 I97 I112 I127 I142 I157">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0.0625</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0.0625</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76:C165 C2:C71" xr:uid="{6E4899FF-3B25-4EE1-B31B-EF5F8A1E414F}">
+      <formula1>$Q$1:$Q$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Timesheet updated by Kavin
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{868298F1-4179-4244-850F-29AD6DC52010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08AE3025-7EFC-4C89-ABF1-B1ECBF89AAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="18" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="647">
   <si>
     <t>Resource Name</t>
   </si>
@@ -2002,6 +2002,12 @@
     <t>IN Progress</t>
   </si>
   <si>
+    <t>Services Implementation</t>
+  </si>
+  <si>
+    <t>Component binding</t>
+  </si>
+  <si>
     <t>Buildinng models and migrations</t>
   </si>
   <si>
@@ -2125,6 +2131,12 @@
     <t>Angular Component Exploration</t>
   </si>
   <si>
+    <t>Assign Review List</t>
+  </si>
+  <si>
+    <t>Completed review list</t>
+  </si>
+  <si>
     <t>Learned Angular &lt;Angular Components&gt;</t>
   </si>
   <si>
@@ -2134,9 +2146,6 @@
     <t>Working on HTML layout(Trainee navbar,View Mom)</t>
   </si>
   <si>
-    <t>Resource Name 7</t>
-  </si>
-  <si>
     <t>Prathima L</t>
   </si>
   <si>
@@ -2185,7 +2194,10 @@
     <t>Meeting with client (rafi)</t>
   </si>
   <si>
-    <t xml:space="preserve">undaerstanding </t>
+    <t xml:space="preserve">Understanding the controller and services in web api </t>
+  </si>
+  <si>
+    <t>understanding and reviewing the models with arul</t>
   </si>
   <si>
     <t>Resource Name 11</t>
@@ -5638,7 +5650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C319A4C-EADA-4641-96D7-D7B692B906C8}">
   <dimension ref="A1:Q165"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -9094,17 +9106,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="A106:A120"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A136:A150"/>
+    <mergeCell ref="A151:A165"/>
     <mergeCell ref="A76:A90"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A45"/>
     <mergeCell ref="A46:A60"/>
     <mergeCell ref="A61:A75"/>
-    <mergeCell ref="A91:A105"/>
-    <mergeCell ref="A106:A120"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A136:A150"/>
-    <mergeCell ref="A151:A165"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I47 I62 I77 I92 I107 I122 I137 I152">
     <cfRule type="cellIs" dxfId="25" priority="12" operator="greaterThan">
@@ -9170,8 +9182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13FBC9E-6B7C-42AF-90E3-40C9ABA19EBC}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="M132" sqref="M132"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="M79" sqref="M79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9326,6 +9338,9 @@
         <f>SUMIFS(F2:F16, C2:C16,H5)</f>
         <v>5.208333333333337E-2</v>
       </c>
+      <c r="M5" t="s">
+        <v>580</v>
+      </c>
       <c r="Q5" t="s">
         <v>513</v>
       </c>
@@ -9355,6 +9370,9 @@
         <f>SUMIFS(F2:F16, C2:C16,H6)</f>
         <v>0</v>
       </c>
+      <c r="M6" t="s">
+        <v>581</v>
+      </c>
       <c r="Q6" t="s">
         <v>512</v>
       </c>
@@ -9362,7 +9380,7 @@
     <row r="7" spans="1:17">
       <c r="A7" s="96"/>
       <c r="B7" s="80" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C7" s="80" t="s">
         <v>504</v>
@@ -9391,7 +9409,7 @@
     <row r="8" spans="1:17">
       <c r="A8" s="96"/>
       <c r="B8" s="80" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>510</v>
@@ -9417,7 +9435,7 @@
     <row r="9" spans="1:17">
       <c r="A9" s="96"/>
       <c r="B9" s="80" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>508</v>
@@ -9463,7 +9481,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="96"/>
       <c r="B11" s="80" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>504</v>
@@ -9483,7 +9501,7 @@
     <row r="12" spans="1:17">
       <c r="A12" s="96"/>
       <c r="B12" s="80" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>504</v>
@@ -9572,7 +9590,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="80" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C17" s="80" t="s">
         <v>508</v>
@@ -9597,7 +9615,7 @@
     <row r="18" spans="1:13">
       <c r="A18" s="96"/>
       <c r="B18" s="80" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C18" s="80" t="s">
         <v>510</v>
@@ -9623,7 +9641,7 @@
     <row r="19" spans="1:13">
       <c r="A19" s="96"/>
       <c r="B19" s="80" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C19" s="80" t="s">
         <v>510</v>
@@ -9649,7 +9667,7 @@
     <row r="20" spans="1:13">
       <c r="A20" s="96"/>
       <c r="B20" s="80" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C20" s="80" t="s">
         <v>516</v>
@@ -9675,7 +9693,7 @@
     <row r="21" spans="1:13">
       <c r="A21" s="96"/>
       <c r="B21" s="80" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C21" s="80" t="s">
         <v>510</v>
@@ -9701,7 +9719,7 @@
     <row r="22" spans="1:13">
       <c r="A22" s="96"/>
       <c r="B22" s="80" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C22" s="80" t="s">
         <v>516</v>
@@ -9727,7 +9745,7 @@
     <row r="23" spans="1:13">
       <c r="A23" s="96"/>
       <c r="B23" s="80" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C23" s="80" t="s">
         <v>504</v>
@@ -9753,7 +9771,7 @@
     <row r="24" spans="1:13">
       <c r="A24" s="96"/>
       <c r="B24" s="80" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C24" s="80" t="s">
         <v>504</v>
@@ -9779,7 +9797,7 @@
     <row r="25" spans="1:13">
       <c r="A25" s="96"/>
       <c r="B25" s="80" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C25" s="80" t="s">
         <v>516</v>
@@ -9799,7 +9817,7 @@
     <row r="26" spans="1:13">
       <c r="A26" s="96"/>
       <c r="B26" s="80" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C26" s="80" t="s">
         <v>504</v>
@@ -9838,7 +9856,7 @@
     <row r="28" spans="1:13">
       <c r="A28" s="96"/>
       <c r="B28" s="80" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C28" s="80" t="s">
         <v>504</v>
@@ -9857,10 +9875,10 @@
     <row r="29" spans="1:13">
       <c r="A29" s="96"/>
       <c r="B29" s="80" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C29" s="80" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D29" s="81">
         <v>23.958333333333332</v>
@@ -9951,13 +9969,13 @@
         <v>0.23611111111111122</v>
       </c>
       <c r="M33" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="96"/>
       <c r="B34" s="80" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C34" s="80" t="s">
         <v>504</v>
@@ -9980,7 +9998,7 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="M34" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -10012,7 +10030,7 @@
     <row r="36" spans="1:13">
       <c r="A36" s="96"/>
       <c r="B36" s="80" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C36" s="80" t="s">
         <v>512</v>
@@ -10064,7 +10082,7 @@
     <row r="38" spans="1:13">
       <c r="A38" s="96"/>
       <c r="B38" s="80" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C38" s="80" t="s">
         <v>504</v>
@@ -10116,7 +10134,7 @@
     <row r="40" spans="1:13">
       <c r="A40" s="96"/>
       <c r="B40" s="80" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C40" s="80" t="s">
         <v>504</v>
@@ -10156,7 +10174,7 @@
     <row r="42" spans="1:13">
       <c r="A42" s="96"/>
       <c r="B42" s="80" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C42" s="80" t="s">
         <v>510</v>
@@ -10175,7 +10193,7 @@
     <row r="43" spans="1:13">
       <c r="A43" s="96"/>
       <c r="B43" s="80" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C43" s="80" t="s">
         <v>504</v>
@@ -10194,7 +10212,7 @@
     <row r="44" spans="1:13">
       <c r="A44" s="96"/>
       <c r="B44" s="80" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C44" s="80" t="s">
         <v>510</v>
@@ -10237,7 +10255,7 @@
         <v>16</v>
       </c>
       <c r="B47" s="80" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C47" s="80" t="s">
         <v>508</v>
@@ -10288,7 +10306,7 @@
         <v>0.35416666666666669</v>
       </c>
       <c r="M48" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -10317,13 +10335,13 @@
         <v>5.902777777777779E-2</v>
       </c>
       <c r="M49" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="96"/>
       <c r="B50" s="80" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C50" s="80" t="s">
         <v>504</v>
@@ -10346,13 +10364,13 @@
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="96"/>
       <c r="B51" s="80" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="C51" s="80" t="s">
         <v>512</v>
@@ -10404,7 +10422,7 @@
     <row r="53" spans="1:13">
       <c r="A53" s="96"/>
       <c r="B53" s="80" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C53" s="80" t="s">
         <v>504</v>
@@ -10430,7 +10448,7 @@
     <row r="54" spans="1:13">
       <c r="A54" s="96"/>
       <c r="B54" s="80" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C54" s="80" t="s">
         <v>504</v>
@@ -10476,7 +10494,7 @@
     <row r="56" spans="1:13">
       <c r="A56" s="96"/>
       <c r="B56" s="80" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C56" s="80" t="s">
         <v>508</v>
@@ -10515,7 +10533,7 @@
     <row r="58" spans="1:13">
       <c r="A58" s="96"/>
       <c r="B58" s="80" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C58" s="80" t="s">
         <v>504</v>
@@ -10534,7 +10552,7 @@
     <row r="59" spans="1:13">
       <c r="A59" s="96"/>
       <c r="B59" s="80" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C59" s="80" t="s">
         <v>504</v>
@@ -10577,7 +10595,7 @@
         <v>17</v>
       </c>
       <c r="B62" s="80" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C62" s="80" t="s">
         <v>508</v>
@@ -10628,7 +10646,7 @@
         <v>0.22222222222222227</v>
       </c>
       <c r="M63" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -10660,10 +10678,10 @@
         <v>299</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:13">
       <c r="A65" s="96"/>
       <c r="B65" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>504</v>
@@ -10686,10 +10704,10 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:13">
       <c r="A66" s="96"/>
       <c r="B66" s="80" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C66" s="80" t="s">
         <v>512</v>
@@ -10712,7 +10730,7 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:13">
       <c r="A67" s="96"/>
       <c r="B67" s="80" t="s">
         <v>518</v>
@@ -10738,10 +10756,10 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:13">
       <c r="A68" s="96"/>
       <c r="B68" s="80" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C68" s="80" t="s">
         <v>504</v>
@@ -10764,7 +10782,7 @@
         <v>6.9444444444444364E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:13">
       <c r="A69" s="96"/>
       <c r="B69" s="80" t="s">
         <v>561</v>
@@ -10790,10 +10808,10 @@
         <v>0.44791666666666663</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:13">
       <c r="A70" s="96"/>
       <c r="B70" s="80" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C70" s="80" t="s">
         <v>508</v>
@@ -10810,10 +10828,10 @@
       </c>
       <c r="I70" s="84"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:13">
       <c r="A71" s="96"/>
       <c r="B71" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="C71" s="80" t="s">
         <v>504</v>
@@ -10830,10 +10848,10 @@
       </c>
       <c r="I71" s="84"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:13">
       <c r="A72" s="96"/>
       <c r="B72" s="80" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C72" s="80" t="s">
         <v>513</v>
@@ -10849,10 +10867,10 @@
         <v>2.0833333333333259E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:13">
       <c r="A73" s="96"/>
       <c r="B73" s="81" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C73" s="80" t="s">
         <v>504</v>
@@ -10868,10 +10886,10 @@
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:13">
       <c r="A74" s="96"/>
       <c r="B74" s="80" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C74" s="80" t="s">
         <v>510</v>
@@ -10887,7 +10905,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:13">
       <c r="A75" s="96"/>
       <c r="B75" s="80"/>
       <c r="C75" s="80"/>
@@ -10898,7 +10916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:13">
       <c r="A76" s="96"/>
       <c r="B76" s="80"/>
       <c r="C76" s="80"/>
@@ -10909,7 +10927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:13">
       <c r="A77" s="96" t="s">
         <v>19</v>
       </c>
@@ -10935,8 +10953,11 @@
       <c r="I77" s="79" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="M77" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="96"/>
       <c r="B78" s="80" t="s">
         <v>551</v>
@@ -10959,10 +10980,13 @@
       </c>
       <c r="I78" s="81">
         <f t="shared" ref="I78" si="31">SUMIFS(F77:F91, C77:C91,H78)</f>
-        <v>0.27361111111111119</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>0.2770833333333334</v>
+      </c>
+      <c r="M78" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="A79" s="96"/>
       <c r="B79" s="80" t="s">
         <v>520</v>
@@ -10985,13 +11009,16 @@
       </c>
       <c r="I79" s="81">
         <f t="shared" ref="I79" si="32">SUMIFS(F77:F91, C77:C91,H79)</f>
-        <v>6.2500000000000111E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M79" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" s="96"/>
       <c r="B80" s="80" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C80" s="80" t="s">
         <v>504</v>
@@ -11037,7 +11064,7 @@
       </c>
       <c r="I81" s="81">
         <f t="shared" ref="I81" si="34">SUMIFS(F77:F91, C77:C91,H81)</f>
-        <v>2.4305555555555469E-2</v>
+        <v>2.7777777777777679E-2</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -11069,7 +11096,7 @@
     <row r="83" spans="1:9">
       <c r="A83" s="96"/>
       <c r="B83" s="80" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="C83" s="80" t="s">
         <v>510</v>
@@ -11095,7 +11122,7 @@
     <row r="84" spans="1:9">
       <c r="A84" s="96"/>
       <c r="B84" s="80" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="C84" s="80" t="s">
         <v>504</v>
@@ -11104,18 +11131,18 @@
         <v>0.59375</v>
       </c>
       <c r="E84" s="81">
-        <v>0.67708333333333337</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="F84" s="81">
         <f t="shared" si="30"/>
-        <v>8.333333333333337E-2</v>
+        <v>0.10069444444444453</v>
       </c>
       <c r="H84" s="78" t="s">
         <v>519</v>
       </c>
       <c r="I84" s="79">
         <f t="shared" ref="I84" si="37">SUM(I78:I83)</f>
-        <v>0.46458333333333346</v>
+        <v>0.47152777777777777</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -11141,78 +11168,70 @@
     <row r="86" spans="1:9">
       <c r="A86" s="96"/>
       <c r="B86" s="80" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C86" s="80" t="s">
         <v>508</v>
       </c>
       <c r="D86" s="81">
-        <v>0.6875</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E86" s="81">
-        <v>0.69444444444444453</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="F86" s="81">
         <f t="shared" si="30"/>
-        <v>6.9444444444445308E-3</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="I86" s="84"/>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="96"/>
       <c r="B87" s="80" t="s">
-        <v>610</v>
+        <v>528</v>
       </c>
       <c r="C87" s="80" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="D87" s="81">
-        <v>0.70138888888888884</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="E87" s="81">
-        <v>0.71527777777777779</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="F87" s="81">
         <f t="shared" si="30"/>
-        <v>1.3888888888888951E-2</v>
+        <v>2.7777777777777679E-2</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="96"/>
       <c r="B88" s="80" t="s">
-        <v>528</v>
+        <v>627</v>
       </c>
       <c r="C88" s="80" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="D88" s="81">
-        <v>0.71875</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="E88" s="81">
-        <v>0.74305555555555547</v>
+        <v>0.86805555555555547</v>
       </c>
       <c r="F88" s="81">
         <f t="shared" si="30"/>
-        <v>2.4305555555555469E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="96"/>
-      <c r="B89" s="80" t="s">
-        <v>623</v>
-      </c>
-      <c r="C89" s="80" t="s">
-        <v>504</v>
-      </c>
-      <c r="D89" s="81">
-        <v>0.74305555555555547</v>
-      </c>
-      <c r="E89" s="81">
-        <v>0.86805555555555547</v>
-      </c>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
       <c r="F89" s="81">
         <f t="shared" si="30"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -11239,7 +11258,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="96" t="s">
-        <v>624</v>
+        <v>20</v>
       </c>
       <c r="B92" s="80" t="s">
         <v>528</v>
@@ -11535,7 +11554,7 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" s="96" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="B107" s="80" t="s">
         <v>526</v>
@@ -11583,7 +11602,7 @@
       </c>
       <c r="I108" s="81">
         <f t="shared" ref="I108" si="45">SUMIFS(F107:F121, C107:C121,H108)</f>
-        <v>0.28819444444444459</v>
+        <v>0.29861111111111133</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -11693,7 +11712,7 @@
     <row r="113" spans="1:13">
       <c r="A113" s="96"/>
       <c r="B113" s="80" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="C113" s="80" t="s">
         <v>504</v>
@@ -11739,13 +11758,13 @@
       </c>
       <c r="I114" s="79">
         <f t="shared" ref="I114" si="51">SUM(I108:I113)</f>
-        <v>0.43541666666666673</v>
+        <v>0.44583333333333347</v>
       </c>
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="96"/>
       <c r="B115" s="80" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="C115" s="80" t="s">
         <v>504</v>
@@ -11810,20 +11829,20 @@
         <v>504</v>
       </c>
       <c r="D118" s="81">
-        <v>0.77083333333333337</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="E118" s="81">
         <v>0.83333333333333337</v>
       </c>
       <c r="F118" s="81">
         <f t="shared" si="30"/>
-        <v>6.25E-2</v>
+        <v>7.2916666666666741E-2</v>
       </c>
     </row>
     <row r="119" spans="1:13">
       <c r="A119" s="96"/>
       <c r="B119" s="80" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C119" s="80" t="s">
         <v>504</v>
@@ -11866,7 +11885,7 @@
         <v>22</v>
       </c>
       <c r="B122" s="80" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="C122" s="80" t="s">
         <v>508</v>
@@ -11888,7 +11907,7 @@
         <v>506</v>
       </c>
       <c r="M122" s="82" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
     </row>
     <row r="123" spans="1:13">
@@ -11917,7 +11936,7 @@
         <v>0.30902777777777785</v>
       </c>
       <c r="M123" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="124" spans="1:13">
@@ -11952,7 +11971,7 @@
     <row r="125" spans="1:13">
       <c r="A125" s="96"/>
       <c r="B125" s="80" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C125" s="80" t="s">
         <v>504</v>
@@ -11978,7 +11997,7 @@
     <row r="126" spans="1:13">
       <c r="A126" s="96"/>
       <c r="B126" s="80" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="C126" s="80" t="s">
         <v>512</v>
@@ -12030,7 +12049,7 @@
     <row r="128" spans="1:13">
       <c r="A128" s="96"/>
       <c r="B128" s="80" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C128" s="80" t="s">
         <v>504</v>
@@ -12056,7 +12075,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="96"/>
       <c r="B129" s="80" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C129" s="80" t="s">
         <v>516</v>
@@ -12082,7 +12101,7 @@
     <row r="130" spans="1:9">
       <c r="A130" s="96"/>
       <c r="B130" s="80" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C130" s="80" t="s">
         <v>508</v>
@@ -12122,7 +12141,7 @@
     <row r="132" spans="1:9">
       <c r="A132" s="96"/>
       <c r="B132" s="80" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C132" s="80" t="s">
         <v>504</v>
@@ -12141,7 +12160,7 @@
     <row r="133" spans="1:9">
       <c r="A133" s="96"/>
       <c r="B133" s="80" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="C133" s="80" t="s">
         <v>508</v>
@@ -12192,7 +12211,7 @@
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="96" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B137" s="80" t="s">
         <v>572</v>
@@ -12240,7 +12259,7 @@
       </c>
       <c r="I138" s="81">
         <f t="shared" ref="I138" si="60">SUMIFS(F137:F151, C137:C151,H138)</f>
-        <v>0.28125</v>
+        <v>0.29166666666666663</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -12272,7 +12291,7 @@
     <row r="140" spans="1:9">
       <c r="A140" s="96"/>
       <c r="B140" s="80" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="C140" s="80" t="s">
         <v>504</v>
@@ -12298,7 +12317,7 @@
     <row r="141" spans="1:9">
       <c r="A141" s="96"/>
       <c r="B141" s="80" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C141" s="80" t="s">
         <v>512</v>
@@ -12350,46 +12369,46 @@
     <row r="143" spans="1:9">
       <c r="A143" s="96"/>
       <c r="B143" s="80" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="C143" s="80" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="D143" s="81">
-        <v>0.65625</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E143" s="81">
-        <v>0.66666666666666663</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="F143" s="81">
         <f t="shared" si="59"/>
-        <v>1.041666666666663E-2</v>
+        <v>5.902777777777779E-2</v>
       </c>
       <c r="H143" s="83" t="s">
         <v>516</v>
       </c>
       <c r="I143" s="81">
         <f t="shared" ref="I143" si="65">SUMIFS(F137:F151, C137:C151,H143)</f>
-        <v>5.2083333333333315E-2</v>
+        <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="96"/>
       <c r="B144" s="80" t="s">
-        <v>578</v>
+        <v>645</v>
       </c>
       <c r="C144" s="80" t="s">
         <v>504</v>
       </c>
       <c r="D144" s="81">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="E144" s="81">
         <v>0.66666666666666663</v>
-      </c>
-      <c r="E144" s="81">
-        <v>0.75</v>
       </c>
       <c r="F144" s="81">
         <f t="shared" si="59"/>
-        <v>8.333333333333337E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="H144" s="78" t="s">
         <v>519</v>
@@ -12488,7 +12507,7 @@
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="96" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="B152" s="80" t="s">
         <v>528</v>
@@ -12784,17 +12803,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">

</xml_diff>

<commit_message>
Updated timesheet by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFEC379D-5804-48A4-94BC-91AE0DD64803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33E4176E-76D4-4F18-A20B-429CAD6915D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="25" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4128" uniqueCount="1023">
   <si>
     <t>Resource Name</t>
   </si>
@@ -3140,12 +3140,24 @@
     <t>started Integration</t>
   </si>
   <si>
-    <t>Creating angular component for topic list</t>
+    <t>Creating angular components for list pages(topic list,course list)</t>
+  </si>
+  <si>
+    <t>Refining styles in angular</t>
   </si>
   <si>
     <t>Refining component pages</t>
   </si>
   <si>
+    <t>angular components refining for list pages</t>
+  </si>
+  <si>
+    <t>Refining all components page</t>
+  </si>
+  <si>
+    <t>Exploration on navbar in angular</t>
+  </si>
+  <si>
     <t>Integrated angular and api ( course list)</t>
   </si>
   <si>
@@ -3206,6 +3218,9 @@
     <t>Angular Component Creating (Profile View for Head, co-ordinator)</t>
   </si>
   <si>
+    <t>Create components for department and course</t>
+  </si>
+  <si>
     <t>Angular Component Refining</t>
   </si>
   <si>
@@ -3221,6 +3236,9 @@
     <t>Angular component creating for View trainer profile ,courselist,topic list</t>
   </si>
   <si>
+    <t>Edit components in angular</t>
+  </si>
+  <si>
     <t>Redefined the created angular components</t>
   </si>
   <si>
@@ -3230,6 +3248,9 @@
     <t>Resolved conflicts and reworked on deleted angular components</t>
   </si>
   <si>
+    <t>Integration on angualar and web api for addreview</t>
+  </si>
+  <si>
     <t>Refining Review services</t>
   </si>
   <si>
@@ -3255,6 +3276,9 @@
   </si>
   <si>
     <t>Intergrating web api and angular (assigned  review)</t>
+  </si>
+  <si>
+    <t>Add department binding</t>
   </si>
   <si>
     <t>binding angular and webapi (topic list page)</t>
@@ -32403,8 +32427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490C0FB0-D79B-42A7-B070-C4769D6ECC67}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36244,8 +36268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E7E2B6-6DCC-4C02-B6AC-CCA2DE26CDBC}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36341,9 +36365,9 @@
       </c>
       <c r="I3" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H3)</f>
-        <v>0.31249999999999994</v>
-      </c>
-      <c r="K3" t="s">
+        <v>0.31944444444444436</v>
+      </c>
+      <c r="K3" s="82" t="s">
         <v>632</v>
       </c>
       <c r="Q3" t="s">
@@ -36376,7 +36400,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="K4" t="s">
-        <v>809</v>
+        <v>958</v>
       </c>
       <c r="Q4" t="s">
         <v>510</v>
@@ -36385,7 +36409,7 @@
     <row r="5" spans="1:17">
       <c r="A5" s="99"/>
       <c r="B5" s="80" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C5" s="80" t="s">
         <v>504</v>
@@ -36405,7 +36429,7 @@
       </c>
       <c r="I5" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H5)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="Q5" t="s">
         <v>513</v>
@@ -36420,21 +36444,21 @@
         <v>512</v>
       </c>
       <c r="D6" s="81">
-        <v>0.44097222222222227</v>
+        <v>0.52430555555555558</v>
       </c>
       <c r="E6" s="81">
-        <v>0.47916666666666669</v>
+        <v>0.55902777777777779</v>
       </c>
       <c r="F6" s="81">
         <f>E6-D6</f>
-        <v>3.819444444444442E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="H6" s="83" t="s">
         <v>513</v>
       </c>
       <c r="I6" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H6)</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>512</v>
@@ -36443,27 +36467,27 @@
     <row r="7" spans="1:17">
       <c r="A7" s="99"/>
       <c r="B7" s="80" t="s">
-        <v>782</v>
+        <v>518</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="D7" s="81">
-        <v>0.47916666666666669</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="E7" s="81">
-        <v>0.52083333333333337</v>
+        <v>0.59375</v>
       </c>
       <c r="F7" s="81">
         <f>E7-D7</f>
-        <v>4.1666666666666685E-2</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="H7" s="83" t="s">
         <v>512</v>
       </c>
       <c r="I7" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H7)</f>
-        <v>3.819444444444442E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="Q7" t="s">
         <v>516</v>
@@ -36472,53 +36496,53 @@
     <row r="8" spans="1:17">
       <c r="A8" s="99"/>
       <c r="B8" s="80" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D8" s="81">
-        <v>0.52083333333333337</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="E8" s="81">
-        <v>0.5625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="F8" s="81">
         <f>E8-D8</f>
-        <v>4.166666666666663E-2</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="H8" s="83" t="s">
         <v>516</v>
       </c>
       <c r="I8" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H8)</f>
-        <v>4.861111111111116E-2</v>
+        <v>3.1250000000000111E-2</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="99"/>
       <c r="B9" s="80" t="s">
-        <v>811</v>
+        <v>960</v>
       </c>
       <c r="C9" s="80" t="s">
         <v>504</v>
       </c>
       <c r="D9" s="81">
-        <v>0.56944444444444442</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E9" s="81">
         <v>0.6875</v>
       </c>
       <c r="F9" s="81">
         <f>E9-D9</f>
-        <v>0.11805555555555558</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="H9" s="78" t="s">
         <v>519</v>
       </c>
       <c r="I9" s="79">
         <f>SUM(I3:I8)</f>
-        <v>0.45486111111111105</v>
+        <v>0.44791666666666669</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -36544,7 +36568,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="99"/>
       <c r="B11" s="80" t="s">
-        <v>812</v>
+        <v>961</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>504</v>
@@ -36553,23 +36577,31 @@
         <v>0.69444444444444453</v>
       </c>
       <c r="E11" s="81">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="F11" s="81">
         <f>E11-D11</f>
-        <v>5.5555555555555469E-2</v>
+        <v>9.7222222222222099E-2</v>
       </c>
       <c r="I11" s="84"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="99"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
+      <c r="B12" s="80" t="s">
+        <v>962</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>510</v>
+      </c>
+      <c r="D12" s="81">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E12" s="81">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F12" s="81">
         <f>E12-D12</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -36621,7 +36653,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C17" s="80" t="s">
         <v>504</v>
@@ -36642,8 +36674,8 @@
       <c r="I17" s="79" t="s">
         <v>506</v>
       </c>
-      <c r="K17" t="s">
-        <v>750</v>
+      <c r="K17" s="82" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -36678,7 +36710,7 @@
     <row r="19" spans="1:11">
       <c r="A19" s="99"/>
       <c r="B19" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="C19" s="80" t="s">
         <v>504</v>
@@ -36730,7 +36762,7 @@
     <row r="21" spans="1:11">
       <c r="A21" s="99"/>
       <c r="B21" t="s">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c r="C21" s="80" t="s">
         <v>504</v>
@@ -36756,7 +36788,7 @@
     <row r="22" spans="1:11">
       <c r="A22" s="99"/>
       <c r="B22" s="80" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="C22" s="80" t="s">
         <v>512</v>
@@ -36834,7 +36866,7 @@
     <row r="25" spans="1:11">
       <c r="A25" s="99"/>
       <c r="B25" s="80" t="s">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c r="C25" s="80" t="s">
         <v>504</v>
@@ -36874,7 +36906,7 @@
     <row r="27" spans="1:11">
       <c r="A27" s="99"/>
       <c r="B27" s="80" t="s">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="C27" s="80" t="s">
         <v>504</v>
@@ -36893,7 +36925,7 @@
     <row r="28" spans="1:11">
       <c r="A28" s="99"/>
       <c r="B28" s="80" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="C28" s="80" t="s">
         <v>504</v>
@@ -36931,7 +36963,7 @@
     <row r="30" spans="1:11">
       <c r="A30" s="99"/>
       <c r="B30" s="80" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="C30" s="80" t="s">
         <v>510</v>
@@ -36950,7 +36982,7 @@
     <row r="31" spans="1:11">
       <c r="A31" s="99"/>
       <c r="B31" s="80" t="s">
-        <v>967</v>
+        <v>971</v>
       </c>
       <c r="C31" s="80" t="s">
         <v>504</v>
@@ -36996,7 +37028,7 @@
     <row r="33" spans="1:11">
       <c r="A33" s="99"/>
       <c r="B33" s="80" t="s">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c r="C33" s="80" t="s">
         <v>504</v>
@@ -37022,7 +37054,7 @@
     <row r="34" spans="1:11">
       <c r="A34" s="99"/>
       <c r="B34" s="18" t="s">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c r="C34" s="80" t="s">
         <v>504</v>
@@ -37096,14 +37128,14 @@
         <f>SUMIFS(F32:F46, C32:C46,H36)</f>
         <v>6.9444444444444198E-3</v>
       </c>
-      <c r="K36" t="s">
-        <v>750</v>
+      <c r="K36" s="82" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="99"/>
       <c r="B37" s="80" t="s">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c r="C37" s="80" t="s">
         <v>504</v>
@@ -37126,7 +37158,7 @@
         <v>4.8611111111111049E-2</v>
       </c>
       <c r="K37" s="80" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -37627,7 +37659,7 @@
     <row r="64" spans="1:11">
       <c r="A64" s="99"/>
       <c r="B64" s="80" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="C64" s="80" t="s">
         <v>504</v>
@@ -37650,13 +37682,13 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="K64" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="99"/>
       <c r="B65" s="80" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>512</v>
@@ -37708,7 +37740,7 @@
     <row r="67" spans="1:11">
       <c r="A67" s="99"/>
       <c r="B67" s="80" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="C67" s="80" t="s">
         <v>513</v>
@@ -37734,7 +37766,7 @@
     <row r="68" spans="1:11">
       <c r="A68" s="99"/>
       <c r="B68" s="80" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="C68" s="80" t="s">
         <v>504</v>
@@ -37939,7 +37971,7 @@
     <row r="79" spans="1:11">
       <c r="A79" s="99"/>
       <c r="B79" s="80" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="C79" s="80" t="s">
         <v>504</v>
@@ -37987,14 +38019,14 @@
         <f>SUMIFS(F77:F91, C77:C91,H80)</f>
         <v>0</v>
       </c>
-      <c r="K80" t="s">
-        <v>845</v>
+      <c r="K80" s="82" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="99"/>
       <c r="B81" s="80" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="C81" s="80" t="s">
         <v>504</v>
@@ -38014,19 +38046,19 @@
       </c>
       <c r="I81" s="81">
         <f>SUMIFS(F77:F91, C77:C91,H81)</f>
-        <v>5.5555555555555469E-2</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="K81" t="s">
-        <v>847</v>
+        <v>983</v>
       </c>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="99"/>
       <c r="B82" s="80" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="C82" s="80" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D82" s="81">
         <v>0.52083333333333337</v>
@@ -38043,7 +38075,7 @@
       </c>
       <c r="I82" s="81">
         <f>SUMIFS(F77:F91, C77:C91,H82)</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -38101,7 +38133,7 @@
     <row r="85" spans="1:11">
       <c r="A85" s="99"/>
       <c r="B85" s="80" t="s">
-        <v>979</v>
+        <v>984</v>
       </c>
       <c r="C85" s="80" t="s">
         <v>504</v>
@@ -38141,7 +38173,7 @@
     <row r="87" spans="1:11">
       <c r="A87" s="99"/>
       <c r="B87" s="80" t="s">
-        <v>980</v>
+        <v>985</v>
       </c>
       <c r="C87" s="80" t="s">
         <v>504</v>
@@ -38206,7 +38238,7 @@
         <v>851</v>
       </c>
       <c r="B92" s="80" t="s">
-        <v>981</v>
+        <v>986</v>
       </c>
       <c r="C92" s="80" t="s">
         <v>504</v>
@@ -38234,7 +38266,7 @@
         <v>808</v>
       </c>
       <c r="C93" s="80" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="D93" s="81">
         <v>0.3888888888888889</v>
@@ -38251,13 +38283,13 @@
       </c>
       <c r="I93" s="81">
         <f>SUMIFS(F92:F106, C92:C106,H93)</f>
-        <v>0.32986111111111105</v>
+        <v>0.32291666666666663</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="99"/>
       <c r="B94" s="80" t="s">
-        <v>982</v>
+        <v>987</v>
       </c>
       <c r="C94" s="80" t="s">
         <v>504</v>
@@ -38277,7 +38309,7 @@
       </c>
       <c r="I94" s="81">
         <f>SUMIFS(F92:F106, C92:C106,H94)</f>
-        <v>1.041666666666663E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -38304,11 +38336,14 @@
       <c r="I95" s="81">
         <v>0</v>
       </c>
+      <c r="K95" s="82" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="99"/>
       <c r="B96" s="80" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="C96" s="80" t="s">
         <v>504</v>
@@ -38328,16 +38363,19 @@
       </c>
       <c r="I96" s="81">
         <f>SUMIFS(F92:F106, C92:C106,H96)</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="K96" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97" s="99"/>
       <c r="B97" s="80" t="s">
         <v>617</v>
       </c>
       <c r="C97" s="80" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D97" s="81">
         <v>0.52083333333333337</v>
@@ -38354,10 +38392,10 @@
       </c>
       <c r="I97" s="81">
         <f>SUMIFS(F92:F106, C92:C106,H97)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98" s="99"/>
       <c r="B98" s="80" t="s">
         <v>518</v>
@@ -38383,13 +38421,13 @@
         <v>4.8611111111111105E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:11">
       <c r="A99" s="99"/>
       <c r="B99" s="80" t="s">
         <v>808</v>
       </c>
       <c r="C99" s="80" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="D99" s="81">
         <v>0.59375</v>
@@ -38409,10 +38447,10 @@
         <v>0.43055555555555541</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:11">
       <c r="A100" s="99"/>
       <c r="B100" s="80" t="s">
-        <v>984</v>
+        <v>990</v>
       </c>
       <c r="C100" s="80" t="s">
         <v>504</v>
@@ -38429,7 +38467,7 @@
       </c>
       <c r="I100" s="84"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:11">
       <c r="A101" s="99"/>
       <c r="B101" s="80" t="s">
         <v>841</v>
@@ -38449,10 +38487,10 @@
       </c>
       <c r="I101" s="84"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:11">
       <c r="A102" s="99"/>
       <c r="B102" s="80" t="s">
-        <v>985</v>
+        <v>991</v>
       </c>
       <c r="C102" s="80" t="s">
         <v>504</v>
@@ -38468,10 +38506,10 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:11">
       <c r="A103" s="99"/>
       <c r="B103" s="80" t="s">
-        <v>986</v>
+        <v>992</v>
       </c>
       <c r="C103" s="80" t="s">
         <v>504</v>
@@ -38486,7 +38524,7 @@
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:11">
       <c r="A104" s="99"/>
       <c r="B104" s="80"/>
       <c r="C104" s="80"/>
@@ -38497,7 +38535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:11">
       <c r="A105" s="99"/>
       <c r="B105" s="80"/>
       <c r="C105" s="80"/>
@@ -38508,7 +38546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:11">
       <c r="A106" s="99"/>
       <c r="B106" s="80"/>
       <c r="C106" s="80"/>
@@ -38519,7 +38557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:11">
       <c r="A107" s="99" t="s">
         <v>631</v>
       </c>
@@ -38545,8 +38583,11 @@
       <c r="I107" s="79" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="108" spans="1:9">
+      <c r="K107" s="82" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108" s="99"/>
       <c r="B108" s="80" t="s">
         <v>528</v>
@@ -38571,11 +38612,14 @@
         <f>SUMIFS(F107:F121, C107:C121,H108)</f>
         <v>0.28819444444444442</v>
       </c>
-    </row>
-    <row r="109" spans="1:9">
+      <c r="K108" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109" s="99"/>
       <c r="B109" s="80" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="C109" s="80" t="s">
         <v>504</v>
@@ -38598,7 +38642,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:11">
       <c r="A110" s="99"/>
       <c r="B110" s="80" t="s">
         <v>792</v>
@@ -38624,10 +38668,10 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:11">
       <c r="A111" s="99"/>
       <c r="B111" s="80" t="s">
-        <v>988</v>
+        <v>995</v>
       </c>
       <c r="C111" s="80" t="s">
         <v>510</v>
@@ -38650,10 +38694,10 @@
         <v>6.9444444444444198E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:11">
       <c r="A112" s="99"/>
       <c r="B112" s="80" t="s">
-        <v>989</v>
+        <v>996</v>
       </c>
       <c r="C112" s="80" t="s">
         <v>512</v>
@@ -38676,7 +38720,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:11">
       <c r="A113" s="99"/>
       <c r="B113" s="80" t="s">
         <v>518</v>
@@ -38702,13 +38746,13 @@
         <v>3.819444444444442E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:11">
       <c r="A114" s="99"/>
       <c r="B114" s="80" t="s">
         <v>528</v>
       </c>
       <c r="C114" s="80" t="s">
-        <v>990</v>
+        <v>997</v>
       </c>
       <c r="D114" s="81">
         <v>0.59375</v>
@@ -38728,10 +38772,10 @@
         <v>0.40277777777777768</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:11">
       <c r="A115" s="99"/>
       <c r="B115" s="80" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
       <c r="C115" s="80" t="s">
         <v>504</v>
@@ -38748,10 +38792,10 @@
       </c>
       <c r="I115" s="84"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:11">
       <c r="A116" s="99"/>
       <c r="B116" s="80" t="s">
-        <v>992</v>
+        <v>999</v>
       </c>
       <c r="C116" s="80" t="s">
         <v>504</v>
@@ -38768,10 +38812,10 @@
       </c>
       <c r="I116" s="84"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:11">
       <c r="A117" s="99"/>
       <c r="B117" s="80" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="C117" s="80" t="s">
         <v>504</v>
@@ -38787,10 +38831,10 @@
         <v>2.777777777777779E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:11">
       <c r="A118" s="99"/>
       <c r="B118" s="18" t="s">
-        <v>994</v>
+        <v>1001</v>
       </c>
       <c r="C118" s="80" t="s">
         <v>504</v>
@@ -38806,10 +38850,10 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:11">
       <c r="A119" s="99"/>
       <c r="B119" s="18" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
       <c r="C119" s="80" t="s">
         <v>504</v>
@@ -38825,7 +38869,7 @@
         <v>7.291666666666663E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:11">
       <c r="A120" s="99"/>
       <c r="B120" s="80"/>
       <c r="C120" s="80"/>
@@ -38836,7 +38880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:11">
       <c r="A121" s="99"/>
       <c r="B121" s="80"/>
       <c r="C121" s="80"/>
@@ -38847,7 +38891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:11">
       <c r="A122" s="99" t="s">
         <v>22</v>
       </c>
@@ -38873,8 +38917,11 @@
       <c r="I122" s="79" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="123" spans="1:9">
+      <c r="K122" s="82" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123" s="99"/>
       <c r="B123" s="80" t="s">
         <v>528</v>
@@ -38899,11 +38946,14 @@
         <f>SUMIFS(F122:F136, C122:C136,H123)</f>
         <v>0.31597222222222221</v>
       </c>
-    </row>
-    <row r="124" spans="1:9">
+      <c r="K123" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124" s="99"/>
       <c r="B124" s="80" t="s">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="C124" s="80" t="s">
         <v>504</v>
@@ -38926,7 +38976,7 @@
         <v>5.902777777777779E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:11">
       <c r="A125" s="99"/>
       <c r="B125" s="80" t="s">
         <v>520</v>
@@ -38952,10 +39002,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:11">
       <c r="A126" s="99"/>
       <c r="B126" s="80" t="s">
-        <v>997</v>
+        <v>1005</v>
       </c>
       <c r="C126" s="80" t="s">
         <v>504</v>
@@ -38978,10 +39028,10 @@
         <v>1.7361111111111049E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:11">
       <c r="A127" s="99"/>
       <c r="B127" s="80" t="s">
-        <v>998</v>
+        <v>1006</v>
       </c>
       <c r="C127" s="80" t="s">
         <v>512</v>
@@ -39004,7 +39054,7 @@
         <v>4.8611111111111049E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:11">
       <c r="A128" s="99"/>
       <c r="B128" s="80" t="s">
         <v>518</v>
@@ -39030,7 +39080,7 @@
         <v>3.4722222222222321E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:11">
       <c r="A129" s="99"/>
       <c r="B129" s="80" t="s">
         <v>528</v>
@@ -39056,10 +39106,10 @@
         <v>0.47569444444444442</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:11">
       <c r="A130" s="99"/>
       <c r="B130" s="80" t="s">
-        <v>999</v>
+        <v>1007</v>
       </c>
       <c r="C130" s="80" t="s">
         <v>508</v>
@@ -39076,10 +39126,10 @@
       </c>
       <c r="I130" s="84"/>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:11">
       <c r="A131" s="99"/>
       <c r="B131" s="80" t="s">
-        <v>1000</v>
+        <v>1008</v>
       </c>
       <c r="C131" s="80" t="s">
         <v>504</v>
@@ -39096,7 +39146,7 @@
       </c>
       <c r="I131" s="84"/>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:11">
       <c r="A132" s="99"/>
       <c r="B132" s="80" t="s">
         <v>521</v>
@@ -39115,10 +39165,10 @@
         <v>6.9444444444445308E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:11">
       <c r="A133" s="99"/>
       <c r="B133" s="80" t="s">
-        <v>1001</v>
+        <v>1009</v>
       </c>
       <c r="C133" s="80" t="s">
         <v>504</v>
@@ -39134,10 +39184,10 @@
         <v>3.472222222222221E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:11">
       <c r="A134" s="99"/>
       <c r="B134" s="80" t="s">
-        <v>1002</v>
+        <v>1010</v>
       </c>
       <c r="C134" s="80" t="s">
         <v>504</v>
@@ -39153,7 +39203,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:11">
       <c r="A135" s="99"/>
       <c r="B135" s="80" t="s">
         <v>889</v>
@@ -39172,10 +39222,10 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:11">
       <c r="A136" s="99"/>
       <c r="B136" s="80" t="s">
-        <v>1003</v>
+        <v>1011</v>
       </c>
       <c r="C136" s="80" t="s">
         <v>504</v>
@@ -39191,7 +39241,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:11">
       <c r="A137" s="99" t="s">
         <v>647</v>
       </c>
@@ -39217,8 +39267,11 @@
       <c r="I137" s="79" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="138" spans="1:9">
+      <c r="K137" s="82" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138" s="99"/>
       <c r="B138" s="80" t="s">
         <v>528</v>
@@ -39243,11 +39296,14 @@
         <f>SUMIFS(F137:F151, C137:C151,H138)</f>
         <v>0.34722222222222221</v>
       </c>
-    </row>
-    <row r="139" spans="1:9">
+      <c r="K138" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139" s="99"/>
       <c r="B139" s="80" t="s">
-        <v>1004</v>
+        <v>1012</v>
       </c>
       <c r="C139" s="80" t="s">
         <v>504</v>
@@ -39270,7 +39326,7 @@
         <v>3.1250000000000056E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:11">
       <c r="A140" s="99"/>
       <c r="B140" s="80" t="s">
         <v>520</v>
@@ -39296,10 +39352,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:11">
       <c r="A141" s="99"/>
       <c r="B141" s="80" t="s">
-        <v>1005</v>
+        <v>1013</v>
       </c>
       <c r="C141" s="80" t="s">
         <v>504</v>
@@ -39322,10 +39378,10 @@
         <v>1.7361111111111049E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:11">
       <c r="A142" s="99"/>
       <c r="B142" s="80" t="s">
-        <v>998</v>
+        <v>1006</v>
       </c>
       <c r="C142" s="80" t="s">
         <v>512</v>
@@ -39348,7 +39404,7 @@
         <v>4.8611111111111049E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:11">
       <c r="A143" s="99"/>
       <c r="B143" s="80" t="s">
         <v>518</v>
@@ -39374,7 +39430,7 @@
         <v>3.8194444444444586E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:11">
       <c r="A144" s="99"/>
       <c r="B144" s="80" t="s">
         <v>528</v>
@@ -39400,10 +39456,10 @@
         <v>0.48263888888888895</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:11">
       <c r="A145" s="99"/>
       <c r="B145" s="80" t="s">
-        <v>1006</v>
+        <v>1014</v>
       </c>
       <c r="C145" s="80" t="s">
         <v>504</v>
@@ -39420,7 +39476,7 @@
       </c>
       <c r="I145" s="84"/>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:11">
       <c r="A146" s="99"/>
       <c r="B146" s="80" t="s">
         <v>521</v>
@@ -39440,10 +39496,10 @@
       </c>
       <c r="I146" s="84"/>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:11">
       <c r="A147" s="99"/>
       <c r="B147" s="80" t="s">
-        <v>1007</v>
+        <v>1015</v>
       </c>
       <c r="C147" s="80" t="s">
         <v>504</v>
@@ -39459,10 +39515,10 @@
         <v>3.472222222222221E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:11">
       <c r="A148" s="99"/>
       <c r="B148" s="80" t="s">
-        <v>1008</v>
+        <v>1016</v>
       </c>
       <c r="C148" s="80" t="s">
         <v>504</v>
@@ -39478,10 +39534,10 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:11">
       <c r="A149" s="99"/>
       <c r="B149" s="80" t="s">
-        <v>1009</v>
+        <v>1017</v>
       </c>
       <c r="C149" s="80" t="s">
         <v>508</v>
@@ -39497,10 +39553,10 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:11">
       <c r="A150" s="99"/>
       <c r="B150" s="80" t="s">
-        <v>1010</v>
+        <v>1018</v>
       </c>
       <c r="C150" s="80" t="s">
         <v>504</v>
@@ -39516,7 +39572,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:11">
       <c r="A151" s="99"/>
       <c r="B151" s="80"/>
       <c r="C151" s="80"/>
@@ -39527,7 +39583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:11">
       <c r="A152" s="99" t="s">
         <v>23</v>
       </c>
@@ -39554,7 +39610,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:11">
       <c r="A153" s="99"/>
       <c r="B153" s="80" t="s">
         <v>528</v>
@@ -39580,10 +39636,10 @@
         <v>0.30208333333333337</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:11">
       <c r="A154" s="99"/>
       <c r="B154" s="80" t="s">
-        <v>987</v>
+        <v>994</v>
       </c>
       <c r="C154" s="80" t="s">
         <v>504</v>
@@ -39605,11 +39661,14 @@
         <f>SUMIFS(F152:F166, C152:C166,H154)</f>
         <v>1.0416666666666685E-2</v>
       </c>
-    </row>
-    <row r="155" spans="1:9">
+      <c r="K154" s="82" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" s="99"/>
       <c r="B155" s="80" t="s">
-        <v>1011</v>
+        <v>1019</v>
       </c>
       <c r="C155" s="80" t="s">
         <v>510</v>
@@ -39631,11 +39690,14 @@
         <f>SUMIFS(F152:F166, C152:C166,H155)</f>
         <v>7.2916666666666685E-2</v>
       </c>
-    </row>
-    <row r="156" spans="1:9">
+      <c r="K155" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156" s="99"/>
       <c r="B156" s="80" t="s">
-        <v>998</v>
+        <v>1006</v>
       </c>
       <c r="C156" s="80" t="s">
         <v>512</v>
@@ -39658,10 +39720,10 @@
         <v>1.7361111111111049E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:11">
       <c r="A157" s="99"/>
       <c r="B157" s="80" t="s">
-        <v>1012</v>
+        <v>1020</v>
       </c>
       <c r="C157" s="80" t="s">
         <v>516</v>
@@ -39684,7 +39746,7 @@
         <v>4.8611111111111049E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:11">
       <c r="A158" s="99"/>
       <c r="B158" s="80" t="s">
         <v>528</v>
@@ -39710,10 +39772,10 @@
         <v>2.083333333333337E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:11">
       <c r="A159" s="99"/>
       <c r="B159" s="80" t="s">
-        <v>1013</v>
+        <v>1021</v>
       </c>
       <c r="C159" s="80" t="s">
         <v>504</v>
@@ -39736,10 +39798,10 @@
         <v>0.47222222222222221</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:11">
       <c r="A160" s="99"/>
       <c r="B160" s="80" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="C160" s="80" t="s">
         <v>504</v>
@@ -39759,7 +39821,7 @@
     <row r="161" spans="1:9">
       <c r="A161" s="99"/>
       <c r="B161" s="80" t="s">
-        <v>1014</v>
+        <v>1022</v>
       </c>
       <c r="C161" s="80" t="s">
         <v>504</v>

</xml_diff>

<commit_message>
Timesheet and Estimattion updated by Arul
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2517008-32DC-40D2-929A-37864500ACA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB400776-14BB-4653-BADF-99EE534C3A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="27" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4903" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4905" uniqueCount="1136">
   <si>
     <t>Resource Name</t>
   </si>
@@ -3496,6 +3496,9 @@
     <t>Helping on angular routing</t>
   </si>
   <si>
+    <t>JWT for Login and session</t>
+  </si>
+  <si>
     <t>client Meeting</t>
   </si>
   <si>
@@ -3505,7 +3508,7 @@
     <t>Refining HTML pages</t>
   </si>
   <si>
-    <t>Web api Service (JWT)</t>
+    <t xml:space="preserve">Web Api Service Discussion </t>
   </si>
   <si>
     <t>working on topiclist(view)</t>
@@ -3568,7 +3571,7 @@
     <t>Resolving Error and Conflit in API</t>
   </si>
   <si>
-    <t>Changes on Angular Page for CourseList and CourseView</t>
+    <t>Changes on Angular Page for CourseList and CourseView and API</t>
   </si>
   <si>
     <t>working on create Course feedback page</t>
@@ -3613,9 +3616,6 @@
     <t>Reworked on add/edit user</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Api Service Discussion </t>
-  </si>
-  <si>
     <t>Tutorial video about JWT</t>
   </si>
   <si>
@@ -3676,7 +3676,7 @@
     <t>Worked on creating schedule page</t>
   </si>
   <si>
-    <t>Session by team member for integration</t>
+    <t>session by team member for integrating and worked on it</t>
   </si>
 </sst>
 </file>
@@ -12422,17 +12422,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="A106:A120"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A136:A150"/>
+    <mergeCell ref="A151:A165"/>
     <mergeCell ref="A76:A90"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A45"/>
     <mergeCell ref="A46:A60"/>
     <mergeCell ref="A61:A75"/>
-    <mergeCell ref="A91:A105"/>
-    <mergeCell ref="A106:A120"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A136:A150"/>
-    <mergeCell ref="A151:A165"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I47 I62 I77 I92 I107 I122 I137 I152">
     <cfRule type="cellIs" dxfId="207" priority="12" operator="greaterThan">
@@ -16191,17 +16191,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="194" priority="12" operator="greaterThan">
@@ -20037,17 +20037,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="181" priority="12" operator="greaterThan">
@@ -23199,17 +23199,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="168" priority="12" operator="greaterThan">
@@ -26282,17 +26282,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="155" priority="12" operator="greaterThan">
@@ -29557,17 +29557,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="142" priority="12" operator="greaterThan">
@@ -33161,17 +33161,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="129" priority="38" operator="greaterThan">
@@ -37002,17 +37002,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="103" priority="25" operator="greaterThan">
@@ -40792,17 +40792,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="77" priority="25" operator="greaterThan">
@@ -44267,17 +44267,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="51" priority="25" operator="greaterThan">
@@ -44394,8 +44394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{339D93A7-2AAE-4B5D-A9CF-16377D578EBD}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44491,7 +44491,7 @@
       </c>
       <c r="I3" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H3)</f>
-        <v>-0.55208333333333326</v>
+        <v>0.23958333333333343</v>
       </c>
       <c r="K3" s="82" t="s">
         <v>632</v>
@@ -44526,7 +44526,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="K4" t="s">
-        <v>958</v>
+        <v>1075</v>
       </c>
       <c r="Q4" t="s">
         <v>510</v>
@@ -44564,7 +44564,7 @@
     <row r="6" spans="1:17">
       <c r="A6" s="99"/>
       <c r="B6" s="80" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C6" s="80" t="s">
         <v>512</v>
@@ -44584,7 +44584,7 @@
       </c>
       <c r="I6" s="81">
         <f>SUMIFS(F2:F16, C2:C16,H6)</f>
-        <v>2.4305555555555469E-2</v>
+        <v>3.4722222222222099E-2</v>
       </c>
       <c r="Q6" t="s">
         <v>512</v>
@@ -44622,7 +44622,7 @@
     <row r="8" spans="1:17">
       <c r="A8" s="99"/>
       <c r="B8" s="80" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C8" s="80" t="s">
         <v>504</v>
@@ -44668,7 +44668,7 @@
       </c>
       <c r="I9" s="79">
         <f>SUM(I3:I8)</f>
-        <v>-0.41736111111111096</v>
+        <v>0.3847222222222223</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -44694,7 +44694,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="99"/>
       <c r="B11" s="80" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C11" s="80" t="s">
         <v>504</v>
@@ -44714,7 +44714,7 @@
     <row r="12" spans="1:17">
       <c r="A12" s="99"/>
       <c r="B12" s="80" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C12" s="80" t="s">
         <v>504</v>
@@ -44722,21 +44722,31 @@
       <c r="D12" s="81">
         <v>0.77083333333333337</v>
       </c>
-      <c r="E12" s="81"/>
+      <c r="E12" s="81">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F12" s="81">
         <f>E12-D12</f>
-        <v>-0.77083333333333337</v>
+        <v>2.0833333333333259E-2</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="99"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
+      <c r="B13" s="80" t="s">
+        <v>528</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>513</v>
+      </c>
+      <c r="D13" s="81">
+        <v>0.84375</v>
+      </c>
+      <c r="E13" s="81">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="F13" s="81">
         <f>E13-D13</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -44805,7 +44815,7 @@
     <row r="18" spans="1:11">
       <c r="A18" s="99"/>
       <c r="B18" s="80" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="C18" s="80" t="s">
         <v>504</v>
@@ -44834,7 +44844,7 @@
     <row r="19" spans="1:11">
       <c r="A19" s="99"/>
       <c r="B19" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C19" s="80" t="s">
         <v>504</v>
@@ -44886,7 +44896,7 @@
     <row r="21" spans="1:11">
       <c r="A21" s="99"/>
       <c r="B21" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C21" s="80" t="s">
         <v>504</v>
@@ -44912,7 +44922,7 @@
     <row r="22" spans="1:11">
       <c r="A22" s="99"/>
       <c r="B22" s="80" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C22" s="80" t="s">
         <v>513</v>
@@ -44938,7 +44948,7 @@
     <row r="23" spans="1:11">
       <c r="A23" s="99"/>
       <c r="B23" s="80" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C23" s="80" t="s">
         <v>512</v>
@@ -44990,7 +45000,7 @@
     <row r="25" spans="1:11">
       <c r="A25" s="99"/>
       <c r="B25" s="80" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C25" s="80" t="s">
         <v>508</v>
@@ -45052,7 +45062,7 @@
     <row r="28" spans="1:11">
       <c r="A28" s="99"/>
       <c r="B28" s="80" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C28" s="80" t="s">
         <v>504</v>
@@ -45071,7 +45081,7 @@
     <row r="29" spans="1:11">
       <c r="A29" s="99"/>
       <c r="B29" s="80" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C29" s="80" t="s">
         <v>504</v>
@@ -45090,7 +45100,7 @@
     <row r="30" spans="1:11">
       <c r="A30" s="99"/>
       <c r="B30" s="80" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C30" s="80" t="s">
         <v>508</v>
@@ -45109,7 +45119,7 @@
     <row r="31" spans="1:11">
       <c r="A31" s="99"/>
       <c r="B31" s="80" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C31" s="80" t="s">
         <v>510</v>
@@ -45155,7 +45165,7 @@
     <row r="33" spans="1:11">
       <c r="A33" s="99"/>
       <c r="B33" s="80" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C33" s="80" t="s">
         <v>504</v>
@@ -45207,7 +45217,7 @@
     <row r="35" spans="1:11">
       <c r="A35" s="99"/>
       <c r="B35" s="80" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C35" s="80" t="s">
         <v>513</v>
@@ -45233,7 +45243,7 @@
     <row r="36" spans="1:11">
       <c r="A36" s="99"/>
       <c r="B36" s="80" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C36" s="80" t="s">
         <v>504</v>
@@ -45428,7 +45438,7 @@
     <row r="48" spans="1:11">
       <c r="A48" s="99"/>
       <c r="B48" s="80" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="C48" s="80" t="s">
         <v>504</v>
@@ -45483,7 +45493,7 @@
     <row r="50" spans="1:11">
       <c r="A50" s="99"/>
       <c r="B50" s="80" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C50" s="80" t="s">
         <v>504</v>
@@ -45587,7 +45597,7 @@
     <row r="54" spans="1:11">
       <c r="A54" s="99"/>
       <c r="B54" s="80" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C54" s="80" t="s">
         <v>504</v>
@@ -45653,7 +45663,7 @@
     <row r="57" spans="1:11">
       <c r="A57" s="99"/>
       <c r="B57" s="80" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C57" s="80" t="s">
         <v>504</v>
@@ -45672,7 +45682,7 @@
     <row r="58" spans="1:11">
       <c r="A58" s="99"/>
       <c r="B58" s="80" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C58" s="80" t="s">
         <v>504</v>
@@ -45694,7 +45704,7 @@
     <row r="59" spans="1:11">
       <c r="A59" s="99"/>
       <c r="B59" s="80" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C59" s="80" t="s">
         <v>508</v>
@@ -45713,7 +45723,7 @@
     <row r="60" spans="1:11">
       <c r="A60" s="99"/>
       <c r="B60" s="80" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="C60" s="80" t="s">
         <v>504</v>
@@ -45732,7 +45742,7 @@
     <row r="61" spans="1:11">
       <c r="A61" s="99"/>
       <c r="B61" s="80" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C61" s="80" t="s">
         <v>504</v>
@@ -45778,7 +45788,7 @@
     <row r="63" spans="1:11">
       <c r="A63" s="99"/>
       <c r="B63" s="80" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="C63" s="80" t="s">
         <v>504</v>
@@ -45830,13 +45840,13 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="K64" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="99"/>
       <c r="B65" s="80" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>504</v>
@@ -45888,7 +45898,7 @@
     <row r="67" spans="1:11">
       <c r="A67" s="99"/>
       <c r="B67" s="80" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C67" s="80" t="s">
         <v>512</v>
@@ -45940,7 +45950,7 @@
     <row r="69" spans="1:11">
       <c r="A69" s="99"/>
       <c r="B69" s="80" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C69" s="80" t="s">
         <v>504</v>
@@ -46006,7 +46016,7 @@
     <row r="72" spans="1:11">
       <c r="A72" s="99"/>
       <c r="B72" s="80" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="C72" s="80" t="s">
         <v>504</v>
@@ -46106,7 +46116,7 @@
     <row r="78" spans="1:11">
       <c r="A78" s="99"/>
       <c r="B78" s="80" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C78" s="80" t="s">
         <v>504</v>
@@ -46158,7 +46168,7 @@
     <row r="80" spans="1:11">
       <c r="A80" s="99"/>
       <c r="B80" s="80" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C80" s="80" t="s">
         <v>504</v>
@@ -46210,7 +46220,7 @@
         <v>2.4305555555555469E-2</v>
       </c>
       <c r="K81" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -46268,7 +46278,7 @@
     <row r="84" spans="1:11">
       <c r="A84" s="99"/>
       <c r="B84" s="80" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C84" s="80" t="s">
         <v>504</v>
@@ -46353,7 +46363,7 @@
     <row r="88" spans="1:11">
       <c r="A88" s="99"/>
       <c r="B88" s="80" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C88" s="80" t="s">
         <v>504</v>
@@ -46372,7 +46382,7 @@
     <row r="89" spans="1:11">
       <c r="A89" s="99"/>
       <c r="B89" s="80" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C89" s="80" t="s">
         <v>504</v>
@@ -46391,7 +46401,7 @@
     <row r="90" spans="1:11">
       <c r="A90" s="99"/>
       <c r="B90" s="80" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C90" s="80" t="s">
         <v>510</v>
@@ -46420,7 +46430,7 @@
         <v>851</v>
       </c>
       <c r="B92" s="80" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C92" s="80" t="s">
         <v>504</v>
@@ -46445,7 +46455,7 @@
     <row r="93" spans="1:11">
       <c r="A93" s="99"/>
       <c r="B93" s="80" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C93" s="80" t="s">
         <v>504</v>
@@ -46471,7 +46481,7 @@
     <row r="94" spans="1:11">
       <c r="A94" s="99"/>
       <c r="B94" s="80" t="s">
-        <v>1114</v>
+        <v>1079</v>
       </c>
       <c r="C94" s="80" t="s">
         <v>504</v>
@@ -46701,7 +46711,7 @@
     <row r="104" spans="1:11">
       <c r="A104" s="99"/>
       <c r="B104" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C104" s="80" t="s">
         <v>508</v>
@@ -46821,7 +46831,7 @@
     <row r="110" spans="1:11">
       <c r="A110" s="99"/>
       <c r="B110" s="80" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C110" s="80" t="s">
         <v>504</v>
@@ -47048,7 +47058,7 @@
     <row r="120" spans="1:11">
       <c r="A120" s="99"/>
       <c r="B120" s="80" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C120" s="80" t="s">
         <v>508</v>
@@ -47379,7 +47389,7 @@
     <row r="134" spans="1:11">
       <c r="A134" s="99"/>
       <c r="B134" s="80" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C134" s="80" t="s">
         <v>508</v>
@@ -47729,7 +47739,7 @@
     <row r="149" spans="1:11">
       <c r="A149" s="99"/>
       <c r="B149" s="80" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C149" s="80" t="s">
         <v>508</v>
@@ -48052,7 +48062,7 @@
     <row r="163" spans="1:9">
       <c r="A163" s="99"/>
       <c r="B163" s="80" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C163" s="80" t="s">
         <v>504</v>
@@ -48111,17 +48121,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">

</xml_diff>

<commit_message>
Timesheet Updated by Asuvath Jahith
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-Timesheet.xlsx
+++ b/Process/Timesheet/PTW-Timesheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspire Intern - Workshop\Year 2022\Q1\To Trainees\Your Project Name\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC8F00B-B74B-4720-9BF8-D9A834314622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F71AD1DF-6726-463A-B88F-9FFB7A7567DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="36" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7317" uniqueCount="1406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7319" uniqueCount="1408">
   <si>
     <t>Resource Name</t>
   </si>
@@ -4454,6 +4454,12 @@
   </si>
   <si>
     <t>Worked on angular and web api integration</t>
+  </si>
+  <si>
+    <t>angular integration</t>
+  </si>
+  <si>
+    <t>working on put and disable in angular</t>
   </si>
   <si>
     <t>Completed Assignment service</t>
@@ -14621,17 +14627,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A91:A105"/>
-    <mergeCell ref="A106:A120"/>
-    <mergeCell ref="A121:A135"/>
-    <mergeCell ref="A136:A150"/>
-    <mergeCell ref="A151:A165"/>
     <mergeCell ref="A76:A90"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A45"/>
     <mergeCell ref="A46:A60"/>
     <mergeCell ref="A61:A75"/>
+    <mergeCell ref="A91:A105"/>
+    <mergeCell ref="A106:A120"/>
+    <mergeCell ref="A121:A135"/>
+    <mergeCell ref="A136:A150"/>
+    <mergeCell ref="A151:A165"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I47 I62 I77 I92 I107 I122 I137 I152">
     <cfRule type="cellIs" dxfId="337" priority="12" operator="greaterThan">
@@ -18390,17 +18396,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="324" priority="12" operator="greaterThan">
@@ -22236,17 +22242,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="311" priority="12" operator="greaterThan">
@@ -25398,17 +25404,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="298" priority="12" operator="greaterThan">
@@ -28481,17 +28487,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="285" priority="12" operator="greaterThan">
@@ -31756,17 +31762,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="272" priority="12" operator="greaterThan">
@@ -35360,17 +35366,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="259" priority="38" operator="greaterThan">
@@ -39201,17 +39207,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="233" priority="25" operator="greaterThan">
@@ -42991,17 +42997,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="207" priority="25" operator="greaterThan">
@@ -46466,17 +46472,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="181" priority="25" operator="greaterThan">
@@ -50333,17 +50339,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="155" priority="25" operator="greaterThan">
@@ -54002,17 +54008,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="129" priority="25" operator="greaterThan">
@@ -57817,17 +57823,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="103" priority="12" operator="greaterThan">
@@ -61330,17 +61336,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="90" priority="12" operator="greaterThan">
@@ -64503,17 +64509,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="77" priority="12" operator="greaterThan">
@@ -67362,17 +67368,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="64" priority="12" operator="greaterThan">
@@ -70233,17 +70239,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="51" priority="12" operator="greaterThan">
@@ -73157,17 +73163,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="38" priority="12" operator="greaterThan">
@@ -76198,17 +76204,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="25" priority="12" operator="greaterThan">
@@ -76274,8 +76280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D66201-6EBC-4FFE-A56D-34F56BDC806E}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -76580,7 +76586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:11">
       <c r="A17" s="102" t="s">
         <v>9</v>
       </c>
@@ -76591,10 +76597,10 @@
         <v>508</v>
       </c>
       <c r="D17" s="81">
-        <v>0.36458333333333331</v>
+        <v>0.34375</v>
       </c>
       <c r="E17" s="81">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="F17" s="81">
         <f>E17-D17</f>
@@ -76607,10 +76613,10 @@
         <v>506</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:11">
       <c r="A18" s="102"/>
       <c r="B18" s="80" t="s">
-        <v>1361</v>
+        <v>664</v>
       </c>
       <c r="C18" s="80" t="s">
         <v>508</v>
@@ -76619,73 +76625,79 @@
         <v>0.375</v>
       </c>
       <c r="E18" s="81">
-        <v>0.39583333333333331</v>
+        <v>0.75</v>
       </c>
       <c r="F18" s="81">
         <f>E18-D18</f>
-        <v>2.0833333333333315E-2</v>
+        <v>0.375</v>
       </c>
       <c r="H18" s="83" t="s">
         <v>504</v>
       </c>
       <c r="I18" s="81">
         <f>SUMIFS(F17:F31, C17:C31,H18)</f>
-        <v>0.16666666666666669</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>0.125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="102"/>
       <c r="B19" t="s">
-        <v>782</v>
+        <v>528</v>
       </c>
       <c r="C19" s="80" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D19" s="81">
-        <v>0.39583333333333331</v>
+        <v>0.8125</v>
       </c>
       <c r="E19" s="81">
-        <v>0.44444444444444442</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F19" s="81">
         <f>E19-D19</f>
-        <v>4.8611111111111105E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H19" s="83" t="s">
         <v>508</v>
       </c>
       <c r="I19" s="81">
         <f>SUMIFS(F17:F31, C17:C31,H19)</f>
-        <v>0.19791666666666674</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="102"/>
       <c r="B20" s="80" t="s">
-        <v>1362</v>
+        <v>1393</v>
       </c>
       <c r="C20" s="80" t="s">
         <v>504</v>
       </c>
       <c r="D20" s="81">
-        <v>0.45833333333333331</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E20" s="81">
-        <v>0.625</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="F20" s="81">
         <f>E20-D20</f>
-        <v>0.16666666666666669</v>
+        <v>0.125</v>
       </c>
       <c r="H20" s="83" t="s">
         <v>510</v>
       </c>
       <c r="I20" s="81">
         <f>SUMIFS(F17:F31, C17:C31,H20)</f>
-        <v>4.8611111111111105E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="102"/>
       <c r="B21" t="s">
         <v>1323</v>
@@ -76694,24 +76706,24 @@
         <v>508</v>
       </c>
       <c r="D21" s="81">
-        <v>0.66666666666666663</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="E21" s="81">
-        <v>0.83333333333333337</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="F21" s="81">
         <f>E21-D21</f>
-        <v>0.16666666666666674</v>
+        <v>4.0972222222222188E-2</v>
       </c>
       <c r="H21" s="83" t="s">
         <v>513</v>
       </c>
       <c r="I21" s="81">
         <f>SUMIFS(F17:F31, C17:C31,H21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="102"/>
       <c r="B22" s="80"/>
       <c r="C22" s="80"/>
@@ -76729,7 +76741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11">
       <c r="A23" s="102"/>
       <c r="B23" s="80"/>
       <c r="C23" s="80"/>
@@ -76747,7 +76759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:11">
       <c r="A24" s="102"/>
       <c r="C24" s="80"/>
       <c r="D24" s="81"/>
@@ -76761,10 +76773,10 @@
       </c>
       <c r="I24" s="79">
         <f>SUM(I18:I23)</f>
-        <v>0.41319444444444453</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>0.5722222222222223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="102"/>
       <c r="B25" s="80"/>
       <c r="C25" s="80"/>
@@ -76776,7 +76788,7 @@
       </c>
       <c r="I25" s="84"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:11">
       <c r="A26" s="102"/>
       <c r="B26" s="80"/>
       <c r="C26" s="80"/>
@@ -76788,7 +76800,7 @@
       </c>
       <c r="I26" s="84"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:11">
       <c r="A27" s="102"/>
       <c r="B27" s="80"/>
       <c r="C27" s="80"/>
@@ -76799,7 +76811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:11">
       <c r="A28" s="102"/>
       <c r="B28" s="80"/>
       <c r="C28" s="80"/>
@@ -76810,7 +76822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:11">
       <c r="A29" s="102"/>
       <c r="B29" s="80"/>
       <c r="C29" s="80"/>
@@ -76821,7 +76833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11">
       <c r="A30" s="102"/>
       <c r="B30" s="80"/>
       <c r="C30" s="80"/>
@@ -76832,7 +76844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:11">
       <c r="A31" s="102"/>
       <c r="B31" s="80"/>
       <c r="C31" s="80"/>
@@ -76843,7 +76855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:11">
       <c r="A32" s="102" t="s">
         <v>13</v>
       </c>
@@ -76873,7 +76885,7 @@
     <row r="33" spans="1:11">
       <c r="A33" s="102"/>
       <c r="B33" s="80" t="s">
-        <v>1392</v>
+        <v>1394</v>
       </c>
       <c r="C33" s="80" t="s">
         <v>504</v>
@@ -76928,7 +76940,7 @@
     <row r="35" spans="1:11">
       <c r="A35" s="102"/>
       <c r="B35" s="80" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
       <c r="C35" s="80" t="s">
         <v>504</v>
@@ -76951,13 +76963,13 @@
         <v>0</v>
       </c>
       <c r="K35" t="s">
-        <v>1394</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="102"/>
       <c r="B36" s="80" t="s">
-        <v>1395</v>
+        <v>1397</v>
       </c>
       <c r="C36" s="80" t="s">
         <v>504</v>
@@ -77375,7 +77387,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="102"/>
       <c r="B63" s="80" t="s">
-        <v>1396</v>
+        <v>1398</v>
       </c>
       <c r="C63" s="80" t="s">
         <v>504</v>
@@ -77427,7 +77439,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="102"/>
       <c r="B65" s="80" t="s">
-        <v>1397</v>
+        <v>1399</v>
       </c>
       <c r="C65" s="80" t="s">
         <v>508</v>
@@ -77505,7 +77517,7 @@
     <row r="68" spans="1:9">
       <c r="A68" s="102"/>
       <c r="B68" s="80" t="s">
-        <v>1398</v>
+        <v>1400</v>
       </c>
       <c r="C68" s="80" t="s">
         <v>504</v>
@@ -77531,7 +77543,7 @@
     <row r="69" spans="1:9">
       <c r="A69" s="102"/>
       <c r="B69" s="80" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="C69" s="80" t="s">
         <v>504</v>
@@ -77597,7 +77609,7 @@
     <row r="72" spans="1:9">
       <c r="A72" s="102"/>
       <c r="B72" s="80" t="s">
-        <v>1400</v>
+        <v>1402</v>
       </c>
       <c r="C72" s="80" t="s">
         <v>504</v>
@@ -77662,7 +77674,7 @@
         <v>19</v>
       </c>
       <c r="B77" s="80" t="s">
-        <v>1401</v>
+        <v>1403</v>
       </c>
       <c r="C77" s="80" t="s">
         <v>508</v>
@@ -79011,7 +79023,7 @@
     <row r="154" spans="1:9">
       <c r="A154" s="102"/>
       <c r="B154" s="80" t="s">
-        <v>1402</v>
+        <v>1404</v>
       </c>
       <c r="C154" s="80" t="s">
         <v>504</v>
@@ -79037,7 +79049,7 @@
     <row r="155" spans="1:9">
       <c r="A155" s="102"/>
       <c r="B155" s="80" t="s">
-        <v>1403</v>
+        <v>1405</v>
       </c>
       <c r="C155" s="80" t="s">
         <v>504</v>
@@ -79115,7 +79127,7 @@
     <row r="158" spans="1:9">
       <c r="A158" s="102"/>
       <c r="B158" s="80" t="s">
-        <v>1404</v>
+        <v>1406</v>
       </c>
       <c r="C158" s="80" t="s">
         <v>504</v>
@@ -79141,7 +79153,7 @@
     <row r="159" spans="1:9">
       <c r="A159" s="102"/>
       <c r="B159" s="80" t="s">
-        <v>1405</v>
+        <v>1407</v>
       </c>
       <c r="C159" s="80" t="s">
         <v>504</v>
@@ -79269,17 +79281,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A92:A106"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A122:A136"/>
-    <mergeCell ref="A137:A151"/>
-    <mergeCell ref="A152:A166"/>
     <mergeCell ref="A77:A91"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A31"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A47:A61"/>
     <mergeCell ref="A62:A76"/>
+    <mergeCell ref="A92:A106"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A122:A136"/>
+    <mergeCell ref="A137:A151"/>
+    <mergeCell ref="A152:A166"/>
   </mergeCells>
   <conditionalFormatting sqref="I3 I18 I33 I48 I63 I78 I93 I108 I123 I138 I153">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">

</xml_diff>